<commit_message>
auto select num of variables for turn and inflow calibration. Format printout message.
</commit_message>
<xml_diff>
--- a/datasets/input_dir_dummy/MatchupTable.xlsx
+++ b/datasets/input_dir_dummy/MatchupTable.xlsx
@@ -546,15 +546,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>23.93</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B3" s="1" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
@@ -571,58 +567,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+Gunbarrel_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>0417) Shallowford Rd &amp; Gunbarrel Rd</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>Synchro_signal.csv</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="N3" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>23.93</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B4" s="1" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -642,31 +602,19 @@
       <c r="G4" s="1" t="n"/>
       <c r="H4" s="1" t="n"/>
       <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="J4" s="1" t="n"/>
       <c r="K4" s="1" t="n"/>
       <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="M4" s="1" t="n"/>
       <c r="N4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="inlineStr">
-        <is>
-          <t>23.93</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B5" s="1" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
@@ -686,31 +634,19 @@
       <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="J5" s="1" t="n"/>
       <c r="K5" s="1" t="n"/>
       <c r="L5" s="1" t="n"/>
-      <c r="M5" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="M5" s="1" t="n"/>
       <c r="N5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="inlineStr">
-        <is>
-          <t>23.93</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B6" s="1" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
@@ -730,31 +666,19 @@
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
       <c r="L6" s="1" t="n"/>
-      <c r="M6" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="M6" s="1" t="n"/>
       <c r="N6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>114.05</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B7" s="1" t="n">
+        <v>114.05</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
@@ -774,31 +698,19 @@
       <c r="G7" s="1" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="J7" s="1" t="n"/>
       <c r="K7" s="1" t="n"/>
       <c r="L7" s="1" t="n"/>
-      <c r="M7" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="M7" s="1" t="n"/>
       <c r="N7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>114.05</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B8" s="1" t="n">
+        <v>114.05</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
@@ -818,31 +730,19 @@
       <c r="G8" s="1" t="n"/>
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J8" s="1" t="n"/>
       <c r="K8" s="1" t="n"/>
       <c r="L8" s="1" t="n"/>
-      <c r="M8" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M8" s="1" t="n"/>
       <c r="N8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>114.05</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B9" s="1" t="n">
+        <v>114.05</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
@@ -862,31 +762,19 @@
       <c r="G9" s="1" t="n"/>
       <c r="H9" s="1" t="n"/>
       <c r="I9" s="1" t="n"/>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J9" s="1" t="n"/>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
-      <c r="M9" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="M9" s="1" t="n"/>
       <c r="N9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>114.05</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B10" s="1" t="n">
+        <v>114.05</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
@@ -906,31 +794,19 @@
       <c r="G10" s="1" t="n"/>
       <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n"/>
-      <c r="J10" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J10" s="1" t="n"/>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
-      <c r="M10" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="M10" s="1" t="n"/>
       <c r="N10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="inlineStr">
-        <is>
-          <t>201.62</t>
-        </is>
-      </c>
-      <c r="C11" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B11" s="1" t="n">
+        <v>201.62</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
@@ -950,31 +826,19 @@
       <c r="G11" s="1" t="n"/>
       <c r="H11" s="1" t="n"/>
       <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="J11" s="1" t="n"/>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
-      <c r="M11" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="M11" s="1" t="n"/>
       <c r="N11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>201.62</t>
-        </is>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B12" s="1" t="n">
+        <v>201.62</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
@@ -994,31 +858,19 @@
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1" t="n"/>
-      <c r="J12" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
-      <c r="M12" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="M12" s="1" t="n"/>
       <c r="N12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>201.62</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B13" s="1" t="n">
+        <v>201.62</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
@@ -1038,31 +890,19 @@
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="n"/>
       <c r="L13" s="1" t="n"/>
-      <c r="M13" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="M13" s="1" t="n"/>
       <c r="N13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>201.62</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B14" s="1" t="n">
+        <v>201.62</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
@@ -1082,31 +922,19 @@
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
-      <c r="J14" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
       <c r="L14" s="1" t="n"/>
-      <c r="M14" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="M14" s="1" t="n"/>
       <c r="N14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>294.05</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B15" s="1" t="n">
+        <v>294.05</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
@@ -1126,31 +954,19 @@
       <c r="G15" s="1" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
-      <c r="J15" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="J15" s="1" t="n"/>
       <c r="K15" s="1" t="n"/>
       <c r="L15" s="1" t="n"/>
-      <c r="M15" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="M15" s="1" t="n"/>
       <c r="N15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>294.05</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B16" s="1" t="n">
+        <v>294.05</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
@@ -1170,31 +986,19 @@
       <c r="G16" s="1" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
-      <c r="J16" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
       <c r="L16" s="1" t="n"/>
-      <c r="M16" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="M16" s="1" t="n"/>
       <c r="N16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>294.05</t>
-        </is>
-      </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B17" s="1" t="n">
+        <v>294.05</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
@@ -1214,31 +1018,19 @@
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
-      <c r="J17" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="M17" s="1" t="n"/>
       <c r="N17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>294.05</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B18" s="1" t="n">
+        <v>294.05</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
@@ -1258,18 +1050,10 @@
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
-      <c r="J18" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
       <c r="L18" s="1" t="n"/>
-      <c r="M18" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="M18" s="1" t="n"/>
       <c r="N18" s="1" t="n"/>
     </row>
     <row r="19">
@@ -1278,15 +1062,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>24.39</t>
-        </is>
-      </c>
-      <c r="C19" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B19" s="1" t="n">
+        <v>24.39</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
@@ -1303,54 +1083,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G19" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+Lifestyle_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H19" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I19" s="1" t="inlineStr">
-        <is>
-          <t>0416) Shallowford Rd &amp; Lifestyle Way</t>
-        </is>
-      </c>
-      <c r="J19" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
+      <c r="G19" s="1" t="n"/>
+      <c r="H19" s="1" t="n"/>
+      <c r="I19" s="1" t="n"/>
+      <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
-      <c r="L19" s="1" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="M19" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="N19" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L19" s="1" t="n"/>
+      <c r="M19" s="1" t="n"/>
+      <c r="N19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>24.39</t>
-        </is>
-      </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B20" s="1" t="n">
+        <v>24.39</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
@@ -1370,31 +1118,19 @@
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
-      <c r="J20" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="J20" s="1" t="n"/>
       <c r="K20" s="1" t="n"/>
       <c r="L20" s="1" t="n"/>
-      <c r="M20" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="M20" s="1" t="n"/>
       <c r="N20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="inlineStr">
-        <is>
-          <t>24.39</t>
-        </is>
-      </c>
-      <c r="C21" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B21" s="1" t="n">
+        <v>24.39</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
@@ -1414,31 +1150,19 @@
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
-      <c r="J21" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="J21" s="1" t="n"/>
       <c r="K21" s="1" t="n"/>
       <c r="L21" s="1" t="n"/>
-      <c r="M21" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>24.39</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B22" s="1" t="n">
+        <v>24.39</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
@@ -1458,31 +1182,19 @@
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
-      <c r="J22" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="J22" s="1" t="n"/>
       <c r="K22" s="1" t="n"/>
       <c r="L22" s="1" t="n"/>
-      <c r="M22" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="M22" s="1" t="n"/>
       <c r="N22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>113.75</t>
-        </is>
-      </c>
-      <c r="C23" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B23" s="1" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
@@ -1502,31 +1214,19 @@
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
-      <c r="J23" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="J23" s="1" t="n"/>
       <c r="K23" s="1" t="n"/>
       <c r="L23" s="1" t="n"/>
-      <c r="M23" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="M23" s="1" t="n"/>
       <c r="N23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>113.75</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B24" s="1" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
@@ -1546,31 +1246,19 @@
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
-      <c r="J24" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J24" s="1" t="n"/>
       <c r="K24" s="1" t="n"/>
       <c r="L24" s="1" t="n"/>
-      <c r="M24" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M24" s="1" t="n"/>
       <c r="N24" s="1" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="inlineStr">
-        <is>
-          <t>113.75</t>
-        </is>
-      </c>
-      <c r="C25" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B25" s="1" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
@@ -1590,31 +1278,19 @@
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
-      <c r="J25" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J25" s="1" t="n"/>
       <c r="K25" s="1" t="n"/>
       <c r="L25" s="1" t="n"/>
-      <c r="M25" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="M25" s="1" t="n"/>
       <c r="N25" s="1" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="inlineStr">
-        <is>
-          <t>113.75</t>
-        </is>
-      </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B26" s="1" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
@@ -1634,31 +1310,19 @@
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n"/>
-      <c r="J26" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J26" s="1" t="n"/>
       <c r="K26" s="1" t="n"/>
       <c r="L26" s="1" t="n"/>
-      <c r="M26" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="M26" s="1" t="n"/>
       <c r="N26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t>204.06</t>
-        </is>
-      </c>
-      <c r="C27" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B27" s="1" t="n">
+        <v>204.06</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
@@ -1678,31 +1342,19 @@
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
       <c r="I27" s="1" t="n"/>
-      <c r="J27" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="J27" s="1" t="n"/>
       <c r="K27" s="1" t="n"/>
       <c r="L27" s="1" t="n"/>
-      <c r="M27" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="M27" s="1" t="n"/>
       <c r="N27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t>204.06</t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B28" s="1" t="n">
+        <v>204.06</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
@@ -1722,31 +1374,19 @@
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
-      <c r="J28" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="J28" s="1" t="n"/>
       <c r="K28" s="1" t="n"/>
       <c r="L28" s="1" t="n"/>
-      <c r="M28" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="M28" s="1" t="n"/>
       <c r="N28" s="1" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="inlineStr">
-        <is>
-          <t>204.06</t>
-        </is>
-      </c>
-      <c r="C29" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B29" s="1" t="n">
+        <v>204.06</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
@@ -1766,31 +1406,19 @@
       <c r="G29" s="1" t="n"/>
       <c r="H29" s="1" t="n"/>
       <c r="I29" s="1" t="n"/>
-      <c r="J29" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="J29" s="1" t="n"/>
       <c r="K29" s="1" t="n"/>
       <c r="L29" s="1" t="n"/>
-      <c r="M29" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="M29" s="1" t="n"/>
       <c r="N29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="inlineStr">
-        <is>
-          <t>204.06</t>
-        </is>
-      </c>
-      <c r="C30" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B30" s="1" t="n">
+        <v>204.06</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
@@ -1810,31 +1438,19 @@
       <c r="G30" s="1" t="n"/>
       <c r="H30" s="1" t="n"/>
       <c r="I30" s="1" t="n"/>
-      <c r="J30" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="J30" s="1" t="n"/>
       <c r="K30" s="1" t="n"/>
       <c r="L30" s="1" t="n"/>
-      <c r="M30" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="M30" s="1" t="n"/>
       <c r="N30" s="1" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="inlineStr">
-        <is>
-          <t>294.03</t>
-        </is>
-      </c>
-      <c r="C31" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B31" s="1" t="n">
+        <v>294.03</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
@@ -1854,31 +1470,19 @@
       <c r="G31" s="1" t="n"/>
       <c r="H31" s="1" t="n"/>
       <c r="I31" s="1" t="n"/>
-      <c r="J31" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="J31" s="1" t="n"/>
       <c r="K31" s="1" t="n"/>
       <c r="L31" s="1" t="n"/>
-      <c r="M31" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="M31" s="1" t="n"/>
       <c r="N31" s="1" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="inlineStr">
-        <is>
-          <t>294.03</t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B32" s="1" t="n">
+        <v>294.03</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
@@ -1898,31 +1502,19 @@
       <c r="G32" s="1" t="n"/>
       <c r="H32" s="1" t="n"/>
       <c r="I32" s="1" t="n"/>
-      <c r="J32" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="J32" s="1" t="n"/>
       <c r="K32" s="1" t="n"/>
       <c r="L32" s="1" t="n"/>
-      <c r="M32" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="M32" s="1" t="n"/>
       <c r="N32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="inlineStr">
-        <is>
-          <t>294.03</t>
-        </is>
-      </c>
-      <c r="C33" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B33" s="1" t="n">
+        <v>294.03</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D33" s="1" t="inlineStr">
         <is>
@@ -1942,31 +1534,19 @@
       <c r="G33" s="1" t="n"/>
       <c r="H33" s="1" t="n"/>
       <c r="I33" s="1" t="n"/>
-      <c r="J33" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="J33" s="1" t="n"/>
       <c r="K33" s="1" t="n"/>
       <c r="L33" s="1" t="n"/>
-      <c r="M33" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="M33" s="1" t="n"/>
       <c r="N33" s="1" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="inlineStr">
-        <is>
-          <t>294.03</t>
-        </is>
-      </c>
-      <c r="C34" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B34" s="1" t="n">
+        <v>294.03</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
@@ -1986,18 +1566,10 @@
       <c r="G34" s="1" t="n"/>
       <c r="H34" s="1" t="n"/>
       <c r="I34" s="1" t="n"/>
-      <c r="J34" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="J34" s="1" t="n"/>
       <c r="K34" s="1" t="n"/>
       <c r="L34" s="1" t="n"/>
-      <c r="M34" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="M34" s="1" t="n"/>
       <c r="N34" s="1" t="n"/>
     </row>
     <row r="35">
@@ -2006,15 +1578,11 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B35" s="1" t="inlineStr">
-        <is>
-          <t>24.22</t>
-        </is>
-      </c>
-      <c r="C35" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B35" s="1" t="n">
+        <v>24.22</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
@@ -2031,42 +1599,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G35" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I35" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J35" s="1" t="n">
-        <v/>
-      </c>
+      <c r="G35" s="1" t="n"/>
+      <c r="H35" s="1" t="n"/>
+      <c r="I35" s="1" t="n"/>
+      <c r="J35" s="1" t="n"/>
       <c r="K35" s="1" t="n"/>
-      <c r="L35" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M35" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N35" s="1" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="L35" s="1" t="n"/>
+      <c r="M35" s="1" t="n"/>
+      <c r="N35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="inlineStr">
-        <is>
-          <t>24.22</t>
-        </is>
-      </c>
-      <c r="C36" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B36" s="1" t="n">
+        <v>24.22</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
@@ -2086,27 +1634,19 @@
       <c r="G36" s="1" t="n"/>
       <c r="H36" s="1" t="n"/>
       <c r="I36" s="1" t="n"/>
-      <c r="J36" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J36" s="1" t="n"/>
       <c r="K36" s="1" t="n"/>
       <c r="L36" s="1" t="n"/>
-      <c r="M36" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M36" s="1" t="n"/>
       <c r="N36" s="1" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="inlineStr">
-        <is>
-          <t>113.88</t>
-        </is>
-      </c>
-      <c r="C37" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B37" s="1" t="n">
+        <v>113.88</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D37" s="1" t="inlineStr">
         <is>
@@ -2126,27 +1666,19 @@
       <c r="G37" s="1" t="n"/>
       <c r="H37" s="1" t="n"/>
       <c r="I37" s="1" t="n"/>
-      <c r="J37" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J37" s="1" t="n"/>
       <c r="K37" s="1" t="n"/>
       <c r="L37" s="1" t="n"/>
-      <c r="M37" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M37" s="1" t="n"/>
       <c r="N37" s="1" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="inlineStr">
-        <is>
-          <t>113.88</t>
-        </is>
-      </c>
-      <c r="C38" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B38" s="1" t="n">
+        <v>113.88</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="inlineStr">
         <is>
@@ -2166,27 +1698,19 @@
       <c r="G38" s="1" t="n"/>
       <c r="H38" s="1" t="n"/>
       <c r="I38" s="1" t="n"/>
-      <c r="J38" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J38" s="1" t="n"/>
       <c r="K38" s="1" t="n"/>
       <c r="L38" s="1" t="n"/>
-      <c r="M38" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M38" s="1" t="n"/>
       <c r="N38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="inlineStr">
-        <is>
-          <t>293.75</t>
-        </is>
-      </c>
-      <c r="C39" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B39" s="1" t="n">
+        <v>293.75</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
@@ -2206,14 +1730,10 @@
       <c r="G39" s="1" t="n"/>
       <c r="H39" s="1" t="n"/>
       <c r="I39" s="1" t="n"/>
-      <c r="J39" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J39" s="1" t="n"/>
       <c r="K39" s="1" t="n"/>
       <c r="L39" s="1" t="n"/>
-      <c r="M39" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M39" s="1" t="n"/>
       <c r="N39" s="1" t="n"/>
     </row>
     <row r="40">
@@ -2222,15 +1742,11 @@
           <t>7</t>
         </is>
       </c>
-      <c r="B40" s="1" t="inlineStr">
-        <is>
-          <t>113.87</t>
-        </is>
-      </c>
-      <c r="C40" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B40" s="1" t="n">
+        <v>113.87</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D40" s="1" t="inlineStr">
         <is>
@@ -2247,42 +1763,22 @@
           <t>thru</t>
         </is>
       </c>
-      <c r="G40" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H40" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I40" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J40" s="1" t="n">
-        <v/>
-      </c>
+      <c r="G40" s="1" t="n"/>
+      <c r="H40" s="1" t="n"/>
+      <c r="I40" s="1" t="n"/>
+      <c r="J40" s="1" t="n"/>
       <c r="K40" s="1" t="n"/>
-      <c r="L40" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M40" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N40" s="1" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="L40" s="1" t="n"/>
+      <c r="M40" s="1" t="n"/>
+      <c r="N40" s="1" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="inlineStr">
-        <is>
-          <t>113.87</t>
-        </is>
-      </c>
-      <c r="C41" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B41" s="1" t="n">
+        <v>113.87</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
@@ -2302,27 +1798,19 @@
       <c r="G41" s="1" t="n"/>
       <c r="H41" s="1" t="n"/>
       <c r="I41" s="1" t="n"/>
-      <c r="J41" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J41" s="1" t="n"/>
       <c r="K41" s="1" t="n"/>
       <c r="L41" s="1" t="n"/>
-      <c r="M41" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M41" s="1" t="n"/>
       <c r="N41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="inlineStr">
-        <is>
-          <t>113.87</t>
-        </is>
-      </c>
-      <c r="C42" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B42" s="1" t="n">
+        <v>113.87</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D42" s="1" t="inlineStr">
         <is>
@@ -2342,27 +1830,19 @@
       <c r="G42" s="1" t="n"/>
       <c r="H42" s="1" t="n"/>
       <c r="I42" s="1" t="n"/>
-      <c r="J42" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J42" s="1" t="n"/>
       <c r="K42" s="1" t="n"/>
       <c r="L42" s="1" t="n"/>
-      <c r="M42" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M42" s="1" t="n"/>
       <c r="N42" s="1" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="inlineStr">
-        <is>
-          <t>193.7</t>
-        </is>
-      </c>
-      <c r="C43" s="1" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="B43" s="1" t="n">
+        <v>193.7</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="D43" s="1" t="inlineStr">
         <is>
@@ -2382,27 +1862,19 @@
       <c r="G43" s="1" t="n"/>
       <c r="H43" s="1" t="n"/>
       <c r="I43" s="1" t="n"/>
-      <c r="J43" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J43" s="1" t="n"/>
       <c r="K43" s="1" t="n"/>
       <c r="L43" s="1" t="n"/>
-      <c r="M43" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M43" s="1" t="n"/>
       <c r="N43" s="1" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="inlineStr">
-        <is>
-          <t>193.7</t>
-        </is>
-      </c>
-      <c r="C44" s="1" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="B44" s="1" t="n">
+        <v>193.7</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="D44" s="1" t="inlineStr">
         <is>
@@ -2422,27 +1894,19 @@
       <c r="G44" s="1" t="n"/>
       <c r="H44" s="1" t="n"/>
       <c r="I44" s="1" t="n"/>
-      <c r="J44" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J44" s="1" t="n"/>
       <c r="K44" s="1" t="n"/>
       <c r="L44" s="1" t="n"/>
-      <c r="M44" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M44" s="1" t="n"/>
       <c r="N44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="inlineStr">
-        <is>
-          <t>193.7</t>
-        </is>
-      </c>
-      <c r="C45" s="1" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="B45" s="1" t="n">
+        <v>193.7</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="inlineStr">
         <is>
@@ -2462,27 +1926,19 @@
       <c r="G45" s="1" t="n"/>
       <c r="H45" s="1" t="n"/>
       <c r="I45" s="1" t="n"/>
-      <c r="J45" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J45" s="1" t="n"/>
       <c r="K45" s="1" t="n"/>
       <c r="L45" s="1" t="n"/>
-      <c r="M45" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M45" s="1" t="n"/>
       <c r="N45" s="1" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="inlineStr">
-        <is>
-          <t>294.04</t>
-        </is>
-      </c>
-      <c r="C46" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B46" s="1" t="n">
+        <v>294.04</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D46" s="1" t="inlineStr">
         <is>
@@ -2502,27 +1958,19 @@
       <c r="G46" s="1" t="n"/>
       <c r="H46" s="1" t="n"/>
       <c r="I46" s="1" t="n"/>
-      <c r="J46" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J46" s="1" t="n"/>
       <c r="K46" s="1" t="n"/>
       <c r="L46" s="1" t="n"/>
-      <c r="M46" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M46" s="1" t="n"/>
       <c r="N46" s="1" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="inlineStr">
-        <is>
-          <t>294.04</t>
-        </is>
-      </c>
-      <c r="C47" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B47" s="1" t="n">
+        <v>294.04</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
@@ -2542,14 +1990,10 @@
       <c r="G47" s="1" t="n"/>
       <c r="H47" s="1" t="n"/>
       <c r="I47" s="1" t="n"/>
-      <c r="J47" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J47" s="1" t="n"/>
       <c r="K47" s="1" t="n"/>
       <c r="L47" s="1" t="n"/>
-      <c r="M47" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M47" s="1" t="n"/>
       <c r="N47" s="1" t="n"/>
     </row>
     <row r="48">
@@ -2558,15 +2002,11 @@
           <t>8</t>
         </is>
       </c>
-      <c r="B48" s="1" t="inlineStr">
-        <is>
-          <t>50.76</t>
-        </is>
-      </c>
-      <c r="C48" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B48" s="1" t="n">
+        <v>50.76</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="D48" s="1" t="inlineStr">
         <is>
@@ -2583,54 +2023,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G48" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+I75N_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H48" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I48" s="1" t="inlineStr">
-        <is>
-          <t>0414) Shallowford Rd &amp; I-75 NB</t>
-        </is>
-      </c>
-      <c r="J48" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
+      <c r="G48" s="1" t="n"/>
+      <c r="H48" s="1" t="n"/>
+      <c r="I48" s="1" t="n"/>
+      <c r="J48" s="1" t="n"/>
       <c r="K48" s="1" t="n"/>
-      <c r="L48" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="M48" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="N48" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L48" s="1" t="n"/>
+      <c r="M48" s="1" t="n"/>
+      <c r="N48" s="1" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="inlineStr">
-        <is>
-          <t>50.76</t>
-        </is>
-      </c>
-      <c r="C49" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B49" s="1" t="n">
+        <v>50.76</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="D49" s="1" t="inlineStr">
         <is>
@@ -2650,31 +2058,19 @@
       <c r="G49" s="1" t="n"/>
       <c r="H49" s="1" t="n"/>
       <c r="I49" s="1" t="n"/>
-      <c r="J49" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="J49" s="1" t="n"/>
       <c r="K49" s="1" t="n"/>
       <c r="L49" s="1" t="n"/>
-      <c r="M49" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="M49" s="1" t="n"/>
       <c r="N49" s="1" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="inlineStr">
-        <is>
-          <t>50.76</t>
-        </is>
-      </c>
-      <c r="C50" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="B50" s="1" t="n">
+        <v>50.76</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="D50" s="1" t="inlineStr">
         <is>
@@ -2694,31 +2090,19 @@
       <c r="G50" s="1" t="n"/>
       <c r="H50" s="1" t="n"/>
       <c r="I50" s="1" t="n"/>
-      <c r="J50" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="J50" s="1" t="n"/>
       <c r="K50" s="1" t="n"/>
       <c r="L50" s="1" t="n"/>
-      <c r="M50" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="M50" s="1" t="n"/>
       <c r="N50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="inlineStr">
-        <is>
-          <t>114.36</t>
-        </is>
-      </c>
-      <c r="C51" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B51" s="1" t="n">
+        <v>114.36</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D51" s="1" t="inlineStr">
         <is>
@@ -2738,31 +2122,19 @@
       <c r="G51" s="1" t="n"/>
       <c r="H51" s="1" t="n"/>
       <c r="I51" s="1" t="n"/>
-      <c r="J51" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="J51" s="1" t="n"/>
       <c r="K51" s="1" t="n"/>
       <c r="L51" s="1" t="n"/>
-      <c r="M51" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="M51" s="1" t="n"/>
       <c r="N51" s="1" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="inlineStr">
-        <is>
-          <t>114.36</t>
-        </is>
-      </c>
-      <c r="C52" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B52" s="1" t="n">
+        <v>114.36</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D52" s="1" t="inlineStr">
         <is>
@@ -2782,31 +2154,19 @@
       <c r="G52" s="1" t="n"/>
       <c r="H52" s="1" t="n"/>
       <c r="I52" s="1" t="n"/>
-      <c r="J52" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J52" s="1" t="n"/>
       <c r="K52" s="1" t="n"/>
       <c r="L52" s="1" t="n"/>
-      <c r="M52" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M52" s="1" t="n"/>
       <c r="N52" s="1" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="inlineStr">
-        <is>
-          <t>114.36</t>
-        </is>
-      </c>
-      <c r="C53" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B53" s="1" t="n">
+        <v>114.36</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D53" s="1" t="inlineStr">
         <is>
@@ -2826,31 +2186,19 @@
       <c r="G53" s="1" t="n"/>
       <c r="H53" s="1" t="n"/>
       <c r="I53" s="1" t="n"/>
-      <c r="J53" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J53" s="1" t="n"/>
       <c r="K53" s="1" t="n"/>
       <c r="L53" s="1" t="n"/>
-      <c r="M53" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="M53" s="1" t="n"/>
       <c r="N53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="inlineStr">
-        <is>
-          <t>296.65</t>
-        </is>
-      </c>
-      <c r="C54" s="1" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="B54" s="1" t="n">
+        <v>296.65</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="D54" s="1" t="inlineStr">
         <is>
@@ -2870,31 +2218,19 @@
       <c r="G54" s="1" t="n"/>
       <c r="H54" s="1" t="n"/>
       <c r="I54" s="1" t="n"/>
-      <c r="J54" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J54" s="1" t="n"/>
       <c r="K54" s="1" t="n"/>
       <c r="L54" s="1" t="n"/>
-      <c r="M54" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="M54" s="1" t="n"/>
       <c r="N54" s="1" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="inlineStr">
-        <is>
-          <t>296.65</t>
-        </is>
-      </c>
-      <c r="C55" s="1" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="B55" s="1" t="n">
+        <v>296.65</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="inlineStr">
         <is>
@@ -2914,18 +2250,10 @@
       <c r="G55" s="1" t="n"/>
       <c r="H55" s="1" t="n"/>
       <c r="I55" s="1" t="n"/>
-      <c r="J55" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="J55" s="1" t="n"/>
       <c r="K55" s="1" t="n"/>
       <c r="L55" s="1" t="n"/>
-      <c r="M55" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="M55" s="1" t="n"/>
       <c r="N55" s="1" t="n"/>
     </row>
     <row r="56">
@@ -2934,15 +2262,11 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B56" s="1" t="inlineStr">
-        <is>
-          <t>111.5</t>
-        </is>
-      </c>
-      <c r="C56" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B56" s="1" t="n">
+        <v>111.5</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D56" s="1" t="inlineStr">
         <is>
@@ -2959,54 +2283,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G56" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+I75S_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H56" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I56" s="1" t="inlineStr">
-        <is>
-          <t>0413) Shallowford Rd &amp; I-75 SB</t>
-        </is>
-      </c>
-      <c r="J56" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="G56" s="1" t="n"/>
+      <c r="H56" s="1" t="n"/>
+      <c r="I56" s="1" t="n"/>
+      <c r="J56" s="1" t="n"/>
       <c r="K56" s="1" t="n"/>
-      <c r="L56" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="M56" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
-      <c r="N56" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L56" s="1" t="n"/>
+      <c r="M56" s="1" t="n"/>
+      <c r="N56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="inlineStr">
-        <is>
-          <t>111.5</t>
-        </is>
-      </c>
-      <c r="C57" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B57" s="1" t="n">
+        <v>111.5</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="inlineStr">
         <is>
@@ -3026,31 +2318,19 @@
       <c r="G57" s="1" t="n"/>
       <c r="H57" s="1" t="n"/>
       <c r="I57" s="1" t="n"/>
-      <c r="J57" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J57" s="1" t="n"/>
       <c r="K57" s="1" t="n"/>
       <c r="L57" s="1" t="n"/>
-      <c r="M57" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M57" s="1" t="n"/>
       <c r="N57" s="1" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="inlineStr">
-        <is>
-          <t>235.09</t>
-        </is>
-      </c>
-      <c r="C58" s="1" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B58" s="1" t="n">
+        <v>235.09</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="D58" s="1" t="inlineStr">
         <is>
@@ -3070,31 +2350,19 @@
       <c r="G58" s="1" t="n"/>
       <c r="H58" s="1" t="n"/>
       <c r="I58" s="1" t="n"/>
-      <c r="J58" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J58" s="1" t="n"/>
       <c r="K58" s="1" t="n"/>
       <c r="L58" s="1" t="n"/>
-      <c r="M58" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="M58" s="1" t="n"/>
       <c r="N58" s="1" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="inlineStr">
-        <is>
-          <t>235.09</t>
-        </is>
-      </c>
-      <c r="C59" s="1" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B59" s="1" t="n">
+        <v>235.09</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="D59" s="1" t="inlineStr">
         <is>
@@ -3114,31 +2382,19 @@
       <c r="G59" s="1" t="n"/>
       <c r="H59" s="1" t="n"/>
       <c r="I59" s="1" t="n"/>
-      <c r="J59" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J59" s="1" t="n"/>
       <c r="K59" s="1" t="n"/>
       <c r="L59" s="1" t="n"/>
-      <c r="M59" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="M59" s="1" t="n"/>
       <c r="N59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="inlineStr">
-        <is>
-          <t>235.09</t>
-        </is>
-      </c>
-      <c r="C60" s="1" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="B60" s="1" t="n">
+        <v>235.09</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="D60" s="1" t="inlineStr">
         <is>
@@ -3158,31 +2414,19 @@
       <c r="G60" s="1" t="n"/>
       <c r="H60" s="1" t="n"/>
       <c r="I60" s="1" t="n"/>
-      <c r="J60" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="J60" s="1" t="n"/>
       <c r="K60" s="1" t="n"/>
       <c r="L60" s="1" t="n"/>
-      <c r="M60" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="M60" s="1" t="n"/>
       <c r="N60" s="1" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="inlineStr">
-        <is>
-          <t>291.99</t>
-        </is>
-      </c>
-      <c r="C61" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B61" s="1" t="n">
+        <v>291.99</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D61" s="1" t="inlineStr">
         <is>
@@ -3202,31 +2446,19 @@
       <c r="G61" s="1" t="n"/>
       <c r="H61" s="1" t="n"/>
       <c r="I61" s="1" t="n"/>
-      <c r="J61" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="J61" s="1" t="n"/>
       <c r="K61" s="1" t="n"/>
       <c r="L61" s="1" t="n"/>
-      <c r="M61" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="M61" s="1" t="n"/>
       <c r="N61" s="1" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="inlineStr">
-        <is>
-          <t>291.99</t>
-        </is>
-      </c>
-      <c r="C62" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B62" s="1" t="n">
+        <v>291.99</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D62" s="1" t="inlineStr">
         <is>
@@ -3246,31 +2478,19 @@
       <c r="G62" s="1" t="n"/>
       <c r="H62" s="1" t="n"/>
       <c r="I62" s="1" t="n"/>
-      <c r="J62" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="J62" s="1" t="n"/>
       <c r="K62" s="1" t="n"/>
       <c r="L62" s="1" t="n"/>
-      <c r="M62" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="M62" s="1" t="n"/>
       <c r="N62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="inlineStr">
-        <is>
-          <t>291.99</t>
-        </is>
-      </c>
-      <c r="C63" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B63" s="1" t="n">
+        <v>291.99</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D63" s="1" t="inlineStr">
         <is>
@@ -3290,18 +2510,10 @@
       <c r="G63" s="1" t="n"/>
       <c r="H63" s="1" t="n"/>
       <c r="I63" s="1" t="n"/>
-      <c r="J63" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="J63" s="1" t="n"/>
       <c r="K63" s="1" t="n"/>
       <c r="L63" s="1" t="n"/>
-      <c r="M63" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="M63" s="1" t="n"/>
       <c r="N63" s="1" t="n"/>
     </row>
     <row r="64">
@@ -3310,15 +2522,11 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B64" s="1" t="inlineStr">
-        <is>
-          <t>25.84</t>
-        </is>
-      </c>
-      <c r="C64" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B64" s="1" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D64" s="1" t="inlineStr">
         <is>
@@ -3335,54 +2543,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G64" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+Napier_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H64" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I64" s="1" t="inlineStr">
-        <is>
-          <t>0415) Shallowford Rd &amp; Napier Rd / Hamilton Place Blvd</t>
-        </is>
-      </c>
-      <c r="J64" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
+      <c r="G64" s="1" t="n"/>
+      <c r="H64" s="1" t="n"/>
+      <c r="I64" s="1" t="n"/>
+      <c r="J64" s="1" t="n"/>
       <c r="K64" s="1" t="n"/>
-      <c r="L64" s="1" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="M64" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="N64" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L64" s="1" t="n"/>
+      <c r="M64" s="1" t="n"/>
+      <c r="N64" s="1" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="inlineStr">
-        <is>
-          <t>25.84</t>
-        </is>
-      </c>
-      <c r="C65" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B65" s="1" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D65" s="1" t="inlineStr">
         <is>
@@ -3402,31 +2578,19 @@
       <c r="G65" s="1" t="n"/>
       <c r="H65" s="1" t="n"/>
       <c r="I65" s="1" t="n"/>
-      <c r="J65" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="J65" s="1" t="n"/>
       <c r="K65" s="1" t="n"/>
       <c r="L65" s="1" t="n"/>
-      <c r="M65" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="M65" s="1" t="n"/>
       <c r="N65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="inlineStr">
-        <is>
-          <t>25.84</t>
-        </is>
-      </c>
-      <c r="C66" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B66" s="1" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D66" s="1" t="inlineStr">
         <is>
@@ -3446,31 +2610,19 @@
       <c r="G66" s="1" t="n"/>
       <c r="H66" s="1" t="n"/>
       <c r="I66" s="1" t="n"/>
-      <c r="J66" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="J66" s="1" t="n"/>
       <c r="K66" s="1" t="n"/>
       <c r="L66" s="1" t="n"/>
-      <c r="M66" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="M66" s="1" t="n"/>
       <c r="N66" s="1" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="inlineStr">
-        <is>
-          <t>25.84</t>
-        </is>
-      </c>
-      <c r="C67" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="B67" s="1" t="n">
+        <v>25.84</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D67" s="1" t="inlineStr">
         <is>
@@ -3490,31 +2642,19 @@
       <c r="G67" s="1" t="n"/>
       <c r="H67" s="1" t="n"/>
       <c r="I67" s="1" t="n"/>
-      <c r="J67" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="J67" s="1" t="n"/>
       <c r="K67" s="1" t="n"/>
       <c r="L67" s="1" t="n"/>
-      <c r="M67" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="M67" s="1" t="n"/>
       <c r="N67" s="1" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
-      <c r="B68" s="1" t="inlineStr">
-        <is>
-          <t>116.65</t>
-        </is>
-      </c>
-      <c r="C68" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="B68" s="1" t="n">
+        <v>116.65</v>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="D68" s="1" t="inlineStr">
         <is>
@@ -3534,31 +2674,19 @@
       <c r="G68" s="1" t="n"/>
       <c r="H68" s="1" t="n"/>
       <c r="I68" s="1" t="n"/>
-      <c r="J68" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="J68" s="1" t="n"/>
       <c r="K68" s="1" t="n"/>
       <c r="L68" s="1" t="n"/>
-      <c r="M68" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="M68" s="1" t="n"/>
       <c r="N68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="inlineStr">
-        <is>
-          <t>116.65</t>
-        </is>
-      </c>
-      <c r="C69" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="B69" s="1" t="n">
+        <v>116.65</v>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="D69" s="1" t="inlineStr">
         <is>
@@ -3578,31 +2706,19 @@
       <c r="G69" s="1" t="n"/>
       <c r="H69" s="1" t="n"/>
       <c r="I69" s="1" t="n"/>
-      <c r="J69" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J69" s="1" t="n"/>
       <c r="K69" s="1" t="n"/>
       <c r="L69" s="1" t="n"/>
-      <c r="M69" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M69" s="1" t="n"/>
       <c r="N69" s="1" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
-      <c r="B70" s="1" t="inlineStr">
-        <is>
-          <t>116.65</t>
-        </is>
-      </c>
-      <c r="C70" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="B70" s="1" t="n">
+        <v>116.65</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="D70" s="1" t="inlineStr">
         <is>
@@ -3622,31 +2738,19 @@
       <c r="G70" s="1" t="n"/>
       <c r="H70" s="1" t="n"/>
       <c r="I70" s="1" t="n"/>
-      <c r="J70" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J70" s="1" t="n"/>
       <c r="K70" s="1" t="n"/>
       <c r="L70" s="1" t="n"/>
-      <c r="M70" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="M70" s="1" t="n"/>
       <c r="N70" s="1" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="inlineStr">
-        <is>
-          <t>116.65</t>
-        </is>
-      </c>
-      <c r="C71" s="1" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="B71" s="1" t="n">
+        <v>116.65</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="D71" s="1" t="inlineStr">
         <is>
@@ -3666,31 +2770,19 @@
       <c r="G71" s="1" t="n"/>
       <c r="H71" s="1" t="n"/>
       <c r="I71" s="1" t="n"/>
-      <c r="J71" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J71" s="1" t="n"/>
       <c r="K71" s="1" t="n"/>
       <c r="L71" s="1" t="n"/>
-      <c r="M71" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="M71" s="1" t="n"/>
       <c r="N71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
-      <c r="B72" s="1" t="inlineStr">
-        <is>
-          <t>202.48</t>
-        </is>
-      </c>
-      <c r="C72" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B72" s="1" t="n">
+        <v>202.48</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D72" s="1" t="inlineStr">
         <is>
@@ -3710,31 +2802,19 @@
       <c r="G72" s="1" t="n"/>
       <c r="H72" s="1" t="n"/>
       <c r="I72" s="1" t="n"/>
-      <c r="J72" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="J72" s="1" t="n"/>
       <c r="K72" s="1" t="n"/>
       <c r="L72" s="1" t="n"/>
-      <c r="M72" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="M72" s="1" t="n"/>
       <c r="N72" s="1" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="inlineStr">
-        <is>
-          <t>202.48</t>
-        </is>
-      </c>
-      <c r="C73" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B73" s="1" t="n">
+        <v>202.48</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D73" s="1" t="inlineStr">
         <is>
@@ -3754,31 +2834,19 @@
       <c r="G73" s="1" t="n"/>
       <c r="H73" s="1" t="n"/>
       <c r="I73" s="1" t="n"/>
-      <c r="J73" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="J73" s="1" t="n"/>
       <c r="K73" s="1" t="n"/>
       <c r="L73" s="1" t="n"/>
-      <c r="M73" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="M73" s="1" t="n"/>
       <c r="N73" s="1" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="inlineStr">
-        <is>
-          <t>202.48</t>
-        </is>
-      </c>
-      <c r="C74" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B74" s="1" t="n">
+        <v>202.48</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D74" s="1" t="inlineStr">
         <is>
@@ -3798,31 +2866,19 @@
       <c r="G74" s="1" t="n"/>
       <c r="H74" s="1" t="n"/>
       <c r="I74" s="1" t="n"/>
-      <c r="J74" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="J74" s="1" t="n"/>
       <c r="K74" s="1" t="n"/>
       <c r="L74" s="1" t="n"/>
-      <c r="M74" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="M74" s="1" t="n"/>
       <c r="N74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="inlineStr">
-        <is>
-          <t>202.48</t>
-        </is>
-      </c>
-      <c r="C75" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B75" s="1" t="n">
+        <v>202.48</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D75" s="1" t="inlineStr">
         <is>
@@ -3842,31 +2898,19 @@
       <c r="G75" s="1" t="n"/>
       <c r="H75" s="1" t="n"/>
       <c r="I75" s="1" t="n"/>
-      <c r="J75" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="J75" s="1" t="n"/>
       <c r="K75" s="1" t="n"/>
       <c r="L75" s="1" t="n"/>
-      <c r="M75" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="M75" s="1" t="n"/>
       <c r="N75" s="1" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="inlineStr">
-        <is>
-          <t>294.22</t>
-        </is>
-      </c>
-      <c r="C76" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B76" s="1" t="n">
+        <v>294.22</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D76" s="1" t="inlineStr">
         <is>
@@ -3886,31 +2930,19 @@
       <c r="G76" s="1" t="n"/>
       <c r="H76" s="1" t="n"/>
       <c r="I76" s="1" t="n"/>
-      <c r="J76" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="J76" s="1" t="n"/>
       <c r="K76" s="1" t="n"/>
       <c r="L76" s="1" t="n"/>
-      <c r="M76" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="M76" s="1" t="n"/>
       <c r="N76" s="1" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="inlineStr">
-        <is>
-          <t>294.22</t>
-        </is>
-      </c>
-      <c r="C77" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B77" s="1" t="n">
+        <v>294.22</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D77" s="1" t="inlineStr">
         <is>
@@ -3930,31 +2962,19 @@
       <c r="G77" s="1" t="n"/>
       <c r="H77" s="1" t="n"/>
       <c r="I77" s="1" t="n"/>
-      <c r="J77" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="J77" s="1" t="n"/>
       <c r="K77" s="1" t="n"/>
       <c r="L77" s="1" t="n"/>
-      <c r="M77" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="M77" s="1" t="n"/>
       <c r="N77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="inlineStr">
-        <is>
-          <t>294.22</t>
-        </is>
-      </c>
-      <c r="C78" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B78" s="1" t="n">
+        <v>294.22</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D78" s="1" t="inlineStr">
         <is>
@@ -3974,31 +2994,19 @@
       <c r="G78" s="1" t="n"/>
       <c r="H78" s="1" t="n"/>
       <c r="I78" s="1" t="n"/>
-      <c r="J78" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="J78" s="1" t="n"/>
       <c r="K78" s="1" t="n"/>
       <c r="L78" s="1" t="n"/>
-      <c r="M78" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="M78" s="1" t="n"/>
       <c r="N78" s="1" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="inlineStr">
-        <is>
-          <t>294.22</t>
-        </is>
-      </c>
-      <c r="C79" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B79" s="1" t="n">
+        <v>294.22</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D79" s="1" t="inlineStr">
         <is>
@@ -4018,18 +3026,10 @@
       <c r="G79" s="1" t="n"/>
       <c r="H79" s="1" t="n"/>
       <c r="I79" s="1" t="n"/>
-      <c r="J79" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="J79" s="1" t="n"/>
       <c r="K79" s="1" t="n"/>
       <c r="L79" s="1" t="n"/>
-      <c r="M79" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="M79" s="1" t="n"/>
       <c r="N79" s="1" t="n"/>
     </row>
     <row r="80">
@@ -4038,15 +3038,11 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B80" s="1" t="inlineStr">
-        <is>
-          <t>22.95</t>
-        </is>
-      </c>
-      <c r="C80" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B80" s="1" t="n">
+        <v>22.95</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D80" s="1" t="inlineStr">
         <is>
@@ -4063,42 +3059,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G80" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H80" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I80" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J80" s="1" t="n">
-        <v/>
-      </c>
+      <c r="G80" s="1" t="n"/>
+      <c r="H80" s="1" t="n"/>
+      <c r="I80" s="1" t="n"/>
+      <c r="J80" s="1" t="n"/>
       <c r="K80" s="1" t="n"/>
-      <c r="L80" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M80" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N80" s="1" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="L80" s="1" t="n"/>
+      <c r="M80" s="1" t="n"/>
+      <c r="N80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="inlineStr">
-        <is>
-          <t>113.22</t>
-        </is>
-      </c>
-      <c r="C81" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B81" s="1" t="n">
+        <v>113.22</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D81" s="1" t="inlineStr">
         <is>
@@ -4118,27 +3094,19 @@
       <c r="G81" s="1" t="n"/>
       <c r="H81" s="1" t="n"/>
       <c r="I81" s="1" t="n"/>
-      <c r="J81" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J81" s="1" t="n"/>
       <c r="K81" s="1" t="n"/>
       <c r="L81" s="1" t="n"/>
-      <c r="M81" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M81" s="1" t="n"/>
       <c r="N81" s="1" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="inlineStr">
-        <is>
-          <t>113.22</t>
-        </is>
-      </c>
-      <c r="C82" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B82" s="1" t="n">
+        <v>113.22</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D82" s="1" t="inlineStr">
         <is>
@@ -4158,27 +3126,19 @@
       <c r="G82" s="1" t="n"/>
       <c r="H82" s="1" t="n"/>
       <c r="I82" s="1" t="n"/>
-      <c r="J82" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J82" s="1" t="n"/>
       <c r="K82" s="1" t="n"/>
       <c r="L82" s="1" t="n"/>
-      <c r="M82" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M82" s="1" t="n"/>
       <c r="N82" s="1" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="inlineStr">
-        <is>
-          <t>113.22</t>
-        </is>
-      </c>
-      <c r="C83" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B83" s="1" t="n">
+        <v>113.22</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D83" s="1" t="inlineStr">
         <is>
@@ -4198,27 +3158,19 @@
       <c r="G83" s="1" t="n"/>
       <c r="H83" s="1" t="n"/>
       <c r="I83" s="1" t="n"/>
-      <c r="J83" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J83" s="1" t="n"/>
       <c r="K83" s="1" t="n"/>
       <c r="L83" s="1" t="n"/>
-      <c r="M83" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M83" s="1" t="n"/>
       <c r="N83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="inlineStr">
-        <is>
-          <t>291.47</t>
-        </is>
-      </c>
-      <c r="C84" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B84" s="1" t="n">
+        <v>291.47</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D84" s="1" t="inlineStr">
         <is>
@@ -4238,27 +3190,19 @@
       <c r="G84" s="1" t="n"/>
       <c r="H84" s="1" t="n"/>
       <c r="I84" s="1" t="n"/>
-      <c r="J84" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J84" s="1" t="n"/>
       <c r="K84" s="1" t="n"/>
       <c r="L84" s="1" t="n"/>
-      <c r="M84" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M84" s="1" t="n"/>
       <c r="N84" s="1" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="inlineStr">
-        <is>
-          <t>291.47</t>
-        </is>
-      </c>
-      <c r="C85" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B85" s="1" t="n">
+        <v>291.47</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D85" s="1" t="inlineStr">
         <is>
@@ -4278,27 +3222,19 @@
       <c r="G85" s="1" t="n"/>
       <c r="H85" s="1" t="n"/>
       <c r="I85" s="1" t="n"/>
-      <c r="J85" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J85" s="1" t="n"/>
       <c r="K85" s="1" t="n"/>
       <c r="L85" s="1" t="n"/>
-      <c r="M85" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M85" s="1" t="n"/>
       <c r="N85" s="1" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
-      <c r="B86" s="1" t="inlineStr">
-        <is>
-          <t>291.47</t>
-        </is>
-      </c>
-      <c r="C86" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B86" s="1" t="n">
+        <v>291.47</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D86" s="1" t="inlineStr">
         <is>
@@ -4318,14 +3254,10 @@
       <c r="G86" s="1" t="n"/>
       <c r="H86" s="1" t="n"/>
       <c r="I86" s="1" t="n"/>
-      <c r="J86" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J86" s="1" t="n"/>
       <c r="K86" s="1" t="n"/>
       <c r="L86" s="1" t="n"/>
-      <c r="M86" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M86" s="1" t="n"/>
       <c r="N86" s="1" t="n"/>
     </row>
     <row r="87">
@@ -4334,15 +3266,11 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B87" s="1" t="inlineStr">
-        <is>
-          <t>23.34</t>
-        </is>
-      </c>
-      <c r="C87" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B87" s="1" t="n">
+        <v>23.34</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D87" s="1" t="inlineStr">
         <is>
@@ -4359,54 +3287,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G87" s="1" t="inlineStr">
-        <is>
-          <t>Shallowford+Amin_07112023.xls</t>
-        </is>
-      </c>
-      <c r="H87" s="1" t="inlineStr">
-        <is>
-          <t>7/11/2023</t>
-        </is>
-      </c>
-      <c r="I87" s="1" t="inlineStr">
-        <is>
-          <t>0412) Shallowford Rd &amp; Shallowford Village Dr / Amin Dr</t>
-        </is>
-      </c>
-      <c r="J87" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
+      <c r="G87" s="1" t="n"/>
+      <c r="H87" s="1" t="n"/>
+      <c r="I87" s="1" t="n"/>
+      <c r="J87" s="1" t="n"/>
       <c r="K87" s="1" t="n"/>
-      <c r="L87" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="M87" s="1" t="inlineStr">
-        <is>
-          <t>NBR</t>
-        </is>
-      </c>
-      <c r="N87" s="1" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
+      <c r="L87" s="1" t="n"/>
+      <c r="M87" s="1" t="n"/>
+      <c r="N87" s="1" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
-      <c r="B88" s="1" t="inlineStr">
-        <is>
-          <t>23.34</t>
-        </is>
-      </c>
-      <c r="C88" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B88" s="1" t="n">
+        <v>23.34</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D88" s="1" t="inlineStr">
         <is>
@@ -4426,31 +3322,19 @@
       <c r="G88" s="1" t="n"/>
       <c r="H88" s="1" t="n"/>
       <c r="I88" s="1" t="n"/>
-      <c r="J88" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="J88" s="1" t="n"/>
       <c r="K88" s="1" t="n"/>
       <c r="L88" s="1" t="n"/>
-      <c r="M88" s="1" t="inlineStr">
-        <is>
-          <t>NBT</t>
-        </is>
-      </c>
+      <c r="M88" s="1" t="n"/>
       <c r="N88" s="1" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
-      <c r="B89" s="1" t="inlineStr">
-        <is>
-          <t>23.34</t>
-        </is>
-      </c>
-      <c r="C89" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B89" s="1" t="n">
+        <v>23.34</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D89" s="1" t="inlineStr">
         <is>
@@ -4470,31 +3354,19 @@
       <c r="G89" s="1" t="n"/>
       <c r="H89" s="1" t="n"/>
       <c r="I89" s="1" t="n"/>
-      <c r="J89" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="J89" s="1" t="n"/>
       <c r="K89" s="1" t="n"/>
       <c r="L89" s="1" t="n"/>
-      <c r="M89" s="1" t="inlineStr">
-        <is>
-          <t>NBL</t>
-        </is>
-      </c>
+      <c r="M89" s="1" t="n"/>
       <c r="N89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="inlineStr">
-        <is>
-          <t>23.34</t>
-        </is>
-      </c>
-      <c r="C90" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B90" s="1" t="n">
+        <v>23.34</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D90" s="1" t="inlineStr">
         <is>
@@ -4514,31 +3386,19 @@
       <c r="G90" s="1" t="n"/>
       <c r="H90" s="1" t="n"/>
       <c r="I90" s="1" t="n"/>
-      <c r="J90" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="J90" s="1" t="n"/>
       <c r="K90" s="1" t="n"/>
       <c r="L90" s="1" t="n"/>
-      <c r="M90" s="1" t="inlineStr">
-        <is>
-          <t>NBU</t>
-        </is>
-      </c>
+      <c r="M90" s="1" t="n"/>
       <c r="N90" s="1" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
-      <c r="B91" s="1" t="inlineStr">
-        <is>
-          <t>114.28</t>
-        </is>
-      </c>
-      <c r="C91" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B91" s="1" t="n">
+        <v>114.28</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D91" s="1" t="inlineStr">
         <is>
@@ -4558,31 +3418,19 @@
       <c r="G91" s="1" t="n"/>
       <c r="H91" s="1" t="n"/>
       <c r="I91" s="1" t="n"/>
-      <c r="J91" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="J91" s="1" t="n"/>
       <c r="K91" s="1" t="n"/>
       <c r="L91" s="1" t="n"/>
-      <c r="M91" s="1" t="inlineStr">
-        <is>
-          <t>EBR</t>
-        </is>
-      </c>
+      <c r="M91" s="1" t="n"/>
       <c r="N91" s="1" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
-      <c r="B92" s="1" t="inlineStr">
-        <is>
-          <t>114.28</t>
-        </is>
-      </c>
-      <c r="C92" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B92" s="1" t="n">
+        <v>114.28</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D92" s="1" t="inlineStr">
         <is>
@@ -4602,31 +3450,19 @@
       <c r="G92" s="1" t="n"/>
       <c r="H92" s="1" t="n"/>
       <c r="I92" s="1" t="n"/>
-      <c r="J92" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="J92" s="1" t="n"/>
       <c r="K92" s="1" t="n"/>
       <c r="L92" s="1" t="n"/>
-      <c r="M92" s="1" t="inlineStr">
-        <is>
-          <t>EBT</t>
-        </is>
-      </c>
+      <c r="M92" s="1" t="n"/>
       <c r="N92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
-      <c r="B93" s="1" t="inlineStr">
-        <is>
-          <t>114.28</t>
-        </is>
-      </c>
-      <c r="C93" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B93" s="1" t="n">
+        <v>114.28</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D93" s="1" t="inlineStr">
         <is>
@@ -4646,31 +3482,19 @@
       <c r="G93" s="1" t="n"/>
       <c r="H93" s="1" t="n"/>
       <c r="I93" s="1" t="n"/>
-      <c r="J93" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="J93" s="1" t="n"/>
       <c r="K93" s="1" t="n"/>
       <c r="L93" s="1" t="n"/>
-      <c r="M93" s="1" t="inlineStr">
-        <is>
-          <t>EBL</t>
-        </is>
-      </c>
+      <c r="M93" s="1" t="n"/>
       <c r="N93" s="1" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="inlineStr">
-        <is>
-          <t>114.28</t>
-        </is>
-      </c>
-      <c r="C94" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B94" s="1" t="n">
+        <v>114.28</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D94" s="1" t="inlineStr">
         <is>
@@ -4690,31 +3514,19 @@
       <c r="G94" s="1" t="n"/>
       <c r="H94" s="1" t="n"/>
       <c r="I94" s="1" t="n"/>
-      <c r="J94" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="J94" s="1" t="n"/>
       <c r="K94" s="1" t="n"/>
       <c r="L94" s="1" t="n"/>
-      <c r="M94" s="1" t="inlineStr">
-        <is>
-          <t>EBU</t>
-        </is>
-      </c>
+      <c r="M94" s="1" t="n"/>
       <c r="N94" s="1" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
-      <c r="B95" s="1" t="inlineStr">
-        <is>
-          <t>201.4</t>
-        </is>
-      </c>
-      <c r="C95" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B95" s="1" t="n">
+        <v>201.4</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D95" s="1" t="inlineStr">
         <is>
@@ -4734,31 +3546,19 @@
       <c r="G95" s="1" t="n"/>
       <c r="H95" s="1" t="n"/>
       <c r="I95" s="1" t="n"/>
-      <c r="J95" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="J95" s="1" t="n"/>
       <c r="K95" s="1" t="n"/>
       <c r="L95" s="1" t="n"/>
-      <c r="M95" s="1" t="inlineStr">
-        <is>
-          <t>SBR</t>
-        </is>
-      </c>
+      <c r="M95" s="1" t="n"/>
       <c r="N95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="inlineStr">
-        <is>
-          <t>201.4</t>
-        </is>
-      </c>
-      <c r="C96" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B96" s="1" t="n">
+        <v>201.4</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D96" s="1" t="inlineStr">
         <is>
@@ -4778,31 +3578,19 @@
       <c r="G96" s="1" t="n"/>
       <c r="H96" s="1" t="n"/>
       <c r="I96" s="1" t="n"/>
-      <c r="J96" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="J96" s="1" t="n"/>
       <c r="K96" s="1" t="n"/>
       <c r="L96" s="1" t="n"/>
-      <c r="M96" s="1" t="inlineStr">
-        <is>
-          <t>SBT</t>
-        </is>
-      </c>
+      <c r="M96" s="1" t="n"/>
       <c r="N96" s="1" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
-      <c r="B97" s="1" t="inlineStr">
-        <is>
-          <t>201.4</t>
-        </is>
-      </c>
-      <c r="C97" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B97" s="1" t="n">
+        <v>201.4</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D97" s="1" t="inlineStr">
         <is>
@@ -4822,31 +3610,19 @@
       <c r="G97" s="1" t="n"/>
       <c r="H97" s="1" t="n"/>
       <c r="I97" s="1" t="n"/>
-      <c r="J97" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="J97" s="1" t="n"/>
       <c r="K97" s="1" t="n"/>
       <c r="L97" s="1" t="n"/>
-      <c r="M97" s="1" t="inlineStr">
-        <is>
-          <t>SBL</t>
-        </is>
-      </c>
+      <c r="M97" s="1" t="n"/>
       <c r="N97" s="1" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="inlineStr">
-        <is>
-          <t>201.4</t>
-        </is>
-      </c>
-      <c r="C98" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B98" s="1" t="n">
+        <v>201.4</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="D98" s="1" t="inlineStr">
         <is>
@@ -4866,31 +3642,19 @@
       <c r="G98" s="1" t="n"/>
       <c r="H98" s="1" t="n"/>
       <c r="I98" s="1" t="n"/>
-      <c r="J98" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="J98" s="1" t="n"/>
       <c r="K98" s="1" t="n"/>
       <c r="L98" s="1" t="n"/>
-      <c r="M98" s="1" t="inlineStr">
-        <is>
-          <t>SBU</t>
-        </is>
-      </c>
+      <c r="M98" s="1" t="n"/>
       <c r="N98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
-      <c r="B99" s="1" t="inlineStr">
-        <is>
-          <t>293.24</t>
-        </is>
-      </c>
-      <c r="C99" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B99" s="1" t="n">
+        <v>293.24</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D99" s="1" t="inlineStr">
         <is>
@@ -4910,31 +3674,19 @@
       <c r="G99" s="1" t="n"/>
       <c r="H99" s="1" t="n"/>
       <c r="I99" s="1" t="n"/>
-      <c r="J99" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="J99" s="1" t="n"/>
       <c r="K99" s="1" t="n"/>
       <c r="L99" s="1" t="n"/>
-      <c r="M99" s="1" t="inlineStr">
-        <is>
-          <t>WBR</t>
-        </is>
-      </c>
+      <c r="M99" s="1" t="n"/>
       <c r="N99" s="1" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
-      <c r="B100" s="1" t="inlineStr">
-        <is>
-          <t>293.24</t>
-        </is>
-      </c>
-      <c r="C100" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B100" s="1" t="n">
+        <v>293.24</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D100" s="1" t="inlineStr">
         <is>
@@ -4954,31 +3706,19 @@
       <c r="G100" s="1" t="n"/>
       <c r="H100" s="1" t="n"/>
       <c r="I100" s="1" t="n"/>
-      <c r="J100" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="J100" s="1" t="n"/>
       <c r="K100" s="1" t="n"/>
       <c r="L100" s="1" t="n"/>
-      <c r="M100" s="1" t="inlineStr">
-        <is>
-          <t>WBT</t>
-        </is>
-      </c>
+      <c r="M100" s="1" t="n"/>
       <c r="N100" s="1" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
-      <c r="B101" s="1" t="inlineStr">
-        <is>
-          <t>293.24</t>
-        </is>
-      </c>
-      <c r="C101" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B101" s="1" t="n">
+        <v>293.24</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D101" s="1" t="inlineStr">
         <is>
@@ -4998,31 +3738,19 @@
       <c r="G101" s="1" t="n"/>
       <c r="H101" s="1" t="n"/>
       <c r="I101" s="1" t="n"/>
-      <c r="J101" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="J101" s="1" t="n"/>
       <c r="K101" s="1" t="n"/>
       <c r="L101" s="1" t="n"/>
-      <c r="M101" s="1" t="inlineStr">
-        <is>
-          <t>WBL</t>
-        </is>
-      </c>
+      <c r="M101" s="1" t="n"/>
       <c r="N101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
-      <c r="B102" s="1" t="inlineStr">
-        <is>
-          <t>293.24</t>
-        </is>
-      </c>
-      <c r="C102" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B102" s="1" t="n">
+        <v>293.24</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D102" s="1" t="inlineStr">
         <is>
@@ -5042,18 +3770,10 @@
       <c r="G102" s="1" t="n"/>
       <c r="H102" s="1" t="n"/>
       <c r="I102" s="1" t="n"/>
-      <c r="J102" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="J102" s="1" t="n"/>
       <c r="K102" s="1" t="n"/>
       <c r="L102" s="1" t="n"/>
-      <c r="M102" s="1" t="inlineStr">
-        <is>
-          <t>WBU</t>
-        </is>
-      </c>
+      <c r="M102" s="1" t="n"/>
       <c r="N102" s="1" t="n"/>
     </row>
     <row r="103">
@@ -5062,15 +3782,11 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B103" s="1" t="inlineStr">
-        <is>
-          <t>24.02</t>
-        </is>
-      </c>
-      <c r="C103" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="B103" s="1" t="n">
+        <v>24.02</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D103" s="1" t="inlineStr">
         <is>
@@ -5087,42 +3803,22 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G103" s="1" t="n">
-        <v/>
-      </c>
-      <c r="H103" s="1" t="n">
-        <v/>
-      </c>
-      <c r="I103" s="1" t="n">
-        <v/>
-      </c>
-      <c r="J103" s="1" t="n">
-        <v/>
-      </c>
+      <c r="G103" s="1" t="n"/>
+      <c r="H103" s="1" t="n"/>
+      <c r="I103" s="1" t="n"/>
+      <c r="J103" s="1" t="n"/>
       <c r="K103" s="1" t="n"/>
-      <c r="L103" s="1" t="n">
-        <v/>
-      </c>
-      <c r="M103" s="1" t="n">
-        <v/>
-      </c>
-      <c r="N103" s="1" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="L103" s="1" t="n"/>
+      <c r="M103" s="1" t="n"/>
+      <c r="N103" s="1" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
-      <c r="B104" s="1" t="inlineStr">
-        <is>
-          <t>114.26</t>
-        </is>
-      </c>
-      <c r="C104" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B104" s="1" t="n">
+        <v>114.26</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D104" s="1" t="inlineStr">
         <is>
@@ -5142,27 +3838,19 @@
       <c r="G104" s="1" t="n"/>
       <c r="H104" s="1" t="n"/>
       <c r="I104" s="1" t="n"/>
-      <c r="J104" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J104" s="1" t="n"/>
       <c r="K104" s="1" t="n"/>
       <c r="L104" s="1" t="n"/>
-      <c r="M104" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M104" s="1" t="n"/>
       <c r="N104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
-      <c r="B105" s="1" t="inlineStr">
-        <is>
-          <t>114.26</t>
-        </is>
-      </c>
-      <c r="C105" s="1" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="B105" s="1" t="n">
+        <v>114.26</v>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="D105" s="1" t="inlineStr">
         <is>
@@ -5182,27 +3870,19 @@
       <c r="G105" s="1" t="n"/>
       <c r="H105" s="1" t="n"/>
       <c r="I105" s="1" t="n"/>
-      <c r="J105" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J105" s="1" t="n"/>
       <c r="K105" s="1" t="n"/>
       <c r="L105" s="1" t="n"/>
-      <c r="M105" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M105" s="1" t="n"/>
       <c r="N105" s="1" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
-      <c r="B106" s="1" t="inlineStr">
-        <is>
-          <t>293.29</t>
-        </is>
-      </c>
-      <c r="C106" s="1" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="B106" s="1" t="n">
+        <v>293.29</v>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="D106" s="1" t="inlineStr">
         <is>
@@ -5222,14 +3902,10 @@
       <c r="G106" s="1" t="n"/>
       <c r="H106" s="1" t="n"/>
       <c r="I106" s="1" t="n"/>
-      <c r="J106" s="1" t="n">
-        <v/>
-      </c>
+      <c r="J106" s="1" t="n"/>
       <c r="K106" s="1" t="n"/>
       <c r="L106" s="1" t="n"/>
-      <c r="M106" s="1" t="n">
-        <v/>
-      </c>
+      <c r="M106" s="1" t="n"/>
       <c r="N106" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not creating SUMO net if exists, currently not enable opendrive to sumo if inc_sumo_net assigned
</commit_message>
<xml_diff>
--- a/datasets/input_dir_dummy/MatchupTable.xlsx
+++ b/datasets/input_dir_dummy/MatchupTable.xlsx
@@ -546,11 +546,15 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>23.93</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>2</v>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>23.93</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
@@ -567,22 +571,58 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
-      <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="n"/>
-      <c r="K3" s="1" t="n"/>
-      <c r="L3" s="1" t="n"/>
-      <c r="M3" s="1" t="n"/>
-      <c r="N3" s="1" t="n"/>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+Gunbarrel_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>0417) Shallowford Rd &amp; Gunbarrel Rd</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t>Synchro_signal.csv</t>
+        </is>
+      </c>
+      <c r="L3" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="M3" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n">
-        <v>23.93</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>2</v>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>23.93</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -602,19 +642,31 @@
       <c r="G4" s="1" t="n"/>
       <c r="H4" s="1" t="n"/>
       <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="n"/>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="K4" s="1" t="n"/>
       <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="n"/>
+      <c r="M4" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="N4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="n">
-        <v>23.93</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2</v>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>23.93</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
@@ -634,19 +686,31 @@
       <c r="G5" s="1" t="n"/>
       <c r="H5" s="1" t="n"/>
       <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="K5" s="1" t="n"/>
       <c r="L5" s="1" t="n"/>
-      <c r="M5" s="1" t="n"/>
+      <c r="M5" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="N5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n">
-        <v>23.93</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>2</v>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>23.93</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
@@ -666,19 +730,31 @@
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="n"/>
       <c r="I6" s="1" t="n"/>
-      <c r="J6" s="1" t="n"/>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="K6" s="1" t="n"/>
       <c r="L6" s="1" t="n"/>
-      <c r="M6" s="1" t="n"/>
+      <c r="M6" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="N6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n">
-        <v>114.05</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>11</v>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>114.05</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
@@ -698,19 +774,31 @@
       <c r="G7" s="1" t="n"/>
       <c r="H7" s="1" t="n"/>
       <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="K7" s="1" t="n"/>
       <c r="L7" s="1" t="n"/>
-      <c r="M7" s="1" t="n"/>
+      <c r="M7" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="N7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n">
-        <v>114.05</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>11</v>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>114.05</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
@@ -730,19 +818,31 @@
       <c r="G8" s="1" t="n"/>
       <c r="H8" s="1" t="n"/>
       <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="n"/>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K8" s="1" t="n"/>
       <c r="L8" s="1" t="n"/>
-      <c r="M8" s="1" t="n"/>
+      <c r="M8" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n">
-        <v>114.05</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>11</v>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>114.05</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
@@ -762,19 +862,31 @@
       <c r="G9" s="1" t="n"/>
       <c r="H9" s="1" t="n"/>
       <c r="I9" s="1" t="n"/>
-      <c r="J9" s="1" t="n"/>
+      <c r="J9" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K9" s="1" t="n"/>
       <c r="L9" s="1" t="n"/>
-      <c r="M9" s="1" t="n"/>
+      <c r="M9" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="N9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n">
-        <v>114.05</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>11</v>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>114.05</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
@@ -794,19 +906,31 @@
       <c r="G10" s="1" t="n"/>
       <c r="H10" s="1" t="n"/>
       <c r="I10" s="1" t="n"/>
-      <c r="J10" s="1" t="n"/>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K10" s="1" t="n"/>
       <c r="L10" s="1" t="n"/>
-      <c r="M10" s="1" t="n"/>
+      <c r="M10" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="N10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="1" t="n">
-        <v>201.62</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>20</v>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>201.62</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
@@ -826,19 +950,31 @@
       <c r="G11" s="1" t="n"/>
       <c r="H11" s="1" t="n"/>
       <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="K11" s="1" t="n"/>
       <c r="L11" s="1" t="n"/>
-      <c r="M11" s="1" t="n"/>
+      <c r="M11" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="N11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n">
-        <v>201.62</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>20</v>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>201.62</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
@@ -858,19 +994,31 @@
       <c r="G12" s="1" t="n"/>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1" t="n"/>
-      <c r="J12" s="1" t="n"/>
+      <c r="J12" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="K12" s="1" t="n"/>
       <c r="L12" s="1" t="n"/>
-      <c r="M12" s="1" t="n"/>
+      <c r="M12" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="N12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n">
-        <v>201.62</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>20</v>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>201.62</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
@@ -890,19 +1038,31 @@
       <c r="G13" s="1" t="n"/>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
-      <c r="J13" s="1" t="n"/>
+      <c r="J13" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="K13" s="1" t="n"/>
       <c r="L13" s="1" t="n"/>
-      <c r="M13" s="1" t="n"/>
+      <c r="M13" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="N13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="1" t="n">
-        <v>201.62</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>20</v>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>201.62</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
@@ -922,19 +1082,31 @@
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
       <c r="I14" s="1" t="n"/>
-      <c r="J14" s="1" t="n"/>
+      <c r="J14" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="K14" s="1" t="n"/>
       <c r="L14" s="1" t="n"/>
-      <c r="M14" s="1" t="n"/>
+      <c r="M14" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="N14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
-      <c r="B15" s="1" t="n">
-        <v>294.05</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>29</v>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>294.05</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
@@ -954,19 +1126,31 @@
       <c r="G15" s="1" t="n"/>
       <c r="H15" s="1" t="n"/>
       <c r="I15" s="1" t="n"/>
-      <c r="J15" s="1" t="n"/>
+      <c r="J15" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="K15" s="1" t="n"/>
       <c r="L15" s="1" t="n"/>
-      <c r="M15" s="1" t="n"/>
+      <c r="M15" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="N15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n"/>
-      <c r="B16" s="1" t="n">
-        <v>294.05</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>29</v>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>294.05</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
@@ -986,19 +1170,31 @@
       <c r="G16" s="1" t="n"/>
       <c r="H16" s="1" t="n"/>
       <c r="I16" s="1" t="n"/>
-      <c r="J16" s="1" t="n"/>
+      <c r="J16" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="K16" s="1" t="n"/>
       <c r="L16" s="1" t="n"/>
-      <c r="M16" s="1" t="n"/>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="N16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n"/>
-      <c r="B17" s="1" t="n">
-        <v>294.05</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>29</v>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>294.05</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
@@ -1018,19 +1214,31 @@
       <c r="G17" s="1" t="n"/>
       <c r="H17" s="1" t="n"/>
       <c r="I17" s="1" t="n"/>
-      <c r="J17" s="1" t="n"/>
+      <c r="J17" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
-      <c r="M17" s="1" t="n"/>
+      <c r="M17" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="N17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="1" t="n">
-        <v>294.05</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>29</v>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>294.05</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
@@ -1050,10 +1258,18 @@
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="n"/>
       <c r="I18" s="1" t="n"/>
-      <c r="J18" s="1" t="n"/>
+      <c r="J18" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="K18" s="1" t="n"/>
       <c r="L18" s="1" t="n"/>
-      <c r="M18" s="1" t="n"/>
+      <c r="M18" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="N18" s="1" t="n"/>
     </row>
     <row r="19">
@@ -1062,11 +1278,15 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B19" s="1" t="n">
-        <v>24.39</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>2</v>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>24.39</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
@@ -1083,22 +1303,54 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G19" s="1" t="n"/>
-      <c r="H19" s="1" t="n"/>
-      <c r="I19" s="1" t="n"/>
-      <c r="J19" s="1" t="n"/>
+      <c r="G19" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+Lifestyle_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H19" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I19" s="1" t="inlineStr">
+        <is>
+          <t>0416) Shallowford Rd &amp; Lifestyle Way</t>
+        </is>
+      </c>
+      <c r="J19" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
       <c r="K19" s="1" t="n"/>
-      <c r="L19" s="1" t="n"/>
-      <c r="M19" s="1" t="n"/>
-      <c r="N19" s="1" t="n"/>
+      <c r="L19" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="M19" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="N19" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="n">
-        <v>24.39</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>2</v>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>24.39</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
@@ -1118,19 +1370,31 @@
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
       <c r="I20" s="1" t="n"/>
-      <c r="J20" s="1" t="n"/>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="K20" s="1" t="n"/>
       <c r="L20" s="1" t="n"/>
-      <c r="M20" s="1" t="n"/>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="N20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="n">
-        <v>24.39</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>2</v>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>24.39</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
@@ -1150,19 +1414,31 @@
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
       <c r="I21" s="1" t="n"/>
-      <c r="J21" s="1" t="n"/>
+      <c r="J21" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="K21" s="1" t="n"/>
       <c r="L21" s="1" t="n"/>
-      <c r="M21" s="1" t="n"/>
+      <c r="M21" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="N21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="1" t="n">
-        <v>24.39</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>2</v>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>24.39</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
@@ -1182,19 +1458,31 @@
       <c r="G22" s="1" t="n"/>
       <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
-      <c r="J22" s="1" t="n"/>
+      <c r="J22" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="K22" s="1" t="n"/>
       <c r="L22" s="1" t="n"/>
-      <c r="M22" s="1" t="n"/>
+      <c r="M22" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="N22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="n">
-        <v>113.75</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>11</v>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>113.75</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
@@ -1214,19 +1502,31 @@
       <c r="G23" s="1" t="n"/>
       <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
-      <c r="J23" s="1" t="n"/>
+      <c r="J23" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="K23" s="1" t="n"/>
       <c r="L23" s="1" t="n"/>
-      <c r="M23" s="1" t="n"/>
+      <c r="M23" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="N23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="1" t="n">
-        <v>113.75</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>11</v>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>113.75</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
@@ -1246,19 +1546,31 @@
       <c r="G24" s="1" t="n"/>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
-      <c r="J24" s="1" t="n"/>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K24" s="1" t="n"/>
       <c r="L24" s="1" t="n"/>
-      <c r="M24" s="1" t="n"/>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N24" s="1" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="1" t="n">
-        <v>113.75</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>11</v>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>113.75</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
@@ -1278,19 +1590,31 @@
       <c r="G25" s="1" t="n"/>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
-      <c r="J25" s="1" t="n"/>
+      <c r="J25" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K25" s="1" t="n"/>
       <c r="L25" s="1" t="n"/>
-      <c r="M25" s="1" t="n"/>
+      <c r="M25" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="N25" s="1" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="1" t="n">
-        <v>113.75</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>11</v>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>113.75</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
@@ -1310,19 +1634,31 @@
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="n"/>
       <c r="I26" s="1" t="n"/>
-      <c r="J26" s="1" t="n"/>
+      <c r="J26" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K26" s="1" t="n"/>
       <c r="L26" s="1" t="n"/>
-      <c r="M26" s="1" t="n"/>
+      <c r="M26" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="N26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="1" t="n">
-        <v>204.06</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>20</v>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>204.06</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
@@ -1342,19 +1678,31 @@
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="n"/>
       <c r="I27" s="1" t="n"/>
-      <c r="J27" s="1" t="n"/>
+      <c r="J27" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="K27" s="1" t="n"/>
       <c r="L27" s="1" t="n"/>
-      <c r="M27" s="1" t="n"/>
+      <c r="M27" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="N27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="1" t="n">
-        <v>204.06</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>20</v>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>204.06</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
@@ -1374,19 +1722,31 @@
       <c r="G28" s="1" t="n"/>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
-      <c r="J28" s="1" t="n"/>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="K28" s="1" t="n"/>
       <c r="L28" s="1" t="n"/>
-      <c r="M28" s="1" t="n"/>
+      <c r="M28" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="N28" s="1" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
-      <c r="B29" s="1" t="n">
-        <v>204.06</v>
-      </c>
-      <c r="C29" s="1" t="n">
-        <v>20</v>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>204.06</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
@@ -1406,19 +1766,31 @@
       <c r="G29" s="1" t="n"/>
       <c r="H29" s="1" t="n"/>
       <c r="I29" s="1" t="n"/>
-      <c r="J29" s="1" t="n"/>
+      <c r="J29" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="K29" s="1" t="n"/>
       <c r="L29" s="1" t="n"/>
-      <c r="M29" s="1" t="n"/>
+      <c r="M29" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="N29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="n">
-        <v>204.06</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>20</v>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>204.06</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
@@ -1438,19 +1810,31 @@
       <c r="G30" s="1" t="n"/>
       <c r="H30" s="1" t="n"/>
       <c r="I30" s="1" t="n"/>
-      <c r="J30" s="1" t="n"/>
+      <c r="J30" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="K30" s="1" t="n"/>
       <c r="L30" s="1" t="n"/>
-      <c r="M30" s="1" t="n"/>
+      <c r="M30" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="N30" s="1" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
-      <c r="B31" s="1" t="n">
-        <v>294.03</v>
-      </c>
-      <c r="C31" s="1" t="n">
-        <v>29</v>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>294.03</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
@@ -1470,19 +1854,31 @@
       <c r="G31" s="1" t="n"/>
       <c r="H31" s="1" t="n"/>
       <c r="I31" s="1" t="n"/>
-      <c r="J31" s="1" t="n"/>
+      <c r="J31" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="K31" s="1" t="n"/>
       <c r="L31" s="1" t="n"/>
-      <c r="M31" s="1" t="n"/>
+      <c r="M31" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="N31" s="1" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n"/>
-      <c r="B32" s="1" t="n">
-        <v>294.03</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>29</v>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>294.03</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
@@ -1502,19 +1898,31 @@
       <c r="G32" s="1" t="n"/>
       <c r="H32" s="1" t="n"/>
       <c r="I32" s="1" t="n"/>
-      <c r="J32" s="1" t="n"/>
+      <c r="J32" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="K32" s="1" t="n"/>
       <c r="L32" s="1" t="n"/>
-      <c r="M32" s="1" t="n"/>
+      <c r="M32" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="N32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
-      <c r="B33" s="1" t="n">
-        <v>294.03</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>29</v>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>294.03</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D33" s="1" t="inlineStr">
         <is>
@@ -1534,19 +1942,31 @@
       <c r="G33" s="1" t="n"/>
       <c r="H33" s="1" t="n"/>
       <c r="I33" s="1" t="n"/>
-      <c r="J33" s="1" t="n"/>
+      <c r="J33" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="K33" s="1" t="n"/>
       <c r="L33" s="1" t="n"/>
-      <c r="M33" s="1" t="n"/>
+      <c r="M33" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="N33" s="1" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
-      <c r="B34" s="1" t="n">
-        <v>294.03</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>29</v>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>294.03</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
@@ -1566,10 +1986,18 @@
       <c r="G34" s="1" t="n"/>
       <c r="H34" s="1" t="n"/>
       <c r="I34" s="1" t="n"/>
-      <c r="J34" s="1" t="n"/>
+      <c r="J34" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="K34" s="1" t="n"/>
       <c r="L34" s="1" t="n"/>
-      <c r="M34" s="1" t="n"/>
+      <c r="M34" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="N34" s="1" t="n"/>
     </row>
     <row r="35">
@@ -1578,11 +2006,15 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B35" s="1" t="n">
-        <v>24.22</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>2</v>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>24.22</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
@@ -1599,22 +2031,42 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G35" s="1" t="n"/>
-      <c r="H35" s="1" t="n"/>
-      <c r="I35" s="1" t="n"/>
-      <c r="J35" s="1" t="n"/>
+      <c r="G35" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J35" s="1" t="n">
+        <v/>
+      </c>
       <c r="K35" s="1" t="n"/>
-      <c r="L35" s="1" t="n"/>
-      <c r="M35" s="1" t="n"/>
-      <c r="N35" s="1" t="n"/>
+      <c r="L35" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N35" s="1" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
-      <c r="B36" s="1" t="n">
-        <v>24.22</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>2</v>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>24.22</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
@@ -1634,19 +2086,27 @@
       <c r="G36" s="1" t="n"/>
       <c r="H36" s="1" t="n"/>
       <c r="I36" s="1" t="n"/>
-      <c r="J36" s="1" t="n"/>
+      <c r="J36" s="1" t="n">
+        <v/>
+      </c>
       <c r="K36" s="1" t="n"/>
       <c r="L36" s="1" t="n"/>
-      <c r="M36" s="1" t="n"/>
+      <c r="M36" s="1" t="n">
+        <v/>
+      </c>
       <c r="N36" s="1" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n"/>
-      <c r="B37" s="1" t="n">
-        <v>113.88</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>11</v>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>113.88</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D37" s="1" t="inlineStr">
         <is>
@@ -1666,19 +2126,27 @@
       <c r="G37" s="1" t="n"/>
       <c r="H37" s="1" t="n"/>
       <c r="I37" s="1" t="n"/>
-      <c r="J37" s="1" t="n"/>
+      <c r="J37" s="1" t="n">
+        <v/>
+      </c>
       <c r="K37" s="1" t="n"/>
       <c r="L37" s="1" t="n"/>
-      <c r="M37" s="1" t="n"/>
+      <c r="M37" s="1" t="n">
+        <v/>
+      </c>
       <c r="N37" s="1" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n"/>
-      <c r="B38" s="1" t="n">
-        <v>113.88</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>11</v>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>113.88</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D38" s="1" t="inlineStr">
         <is>
@@ -1698,19 +2166,27 @@
       <c r="G38" s="1" t="n"/>
       <c r="H38" s="1" t="n"/>
       <c r="I38" s="1" t="n"/>
-      <c r="J38" s="1" t="n"/>
+      <c r="J38" s="1" t="n">
+        <v/>
+      </c>
       <c r="K38" s="1" t="n"/>
       <c r="L38" s="1" t="n"/>
-      <c r="M38" s="1" t="n"/>
+      <c r="M38" s="1" t="n">
+        <v/>
+      </c>
       <c r="N38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n"/>
-      <c r="B39" s="1" t="n">
-        <v>293.75</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>29</v>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>293.75</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
@@ -1730,10 +2206,14 @@
       <c r="G39" s="1" t="n"/>
       <c r="H39" s="1" t="n"/>
       <c r="I39" s="1" t="n"/>
-      <c r="J39" s="1" t="n"/>
+      <c r="J39" s="1" t="n">
+        <v/>
+      </c>
       <c r="K39" s="1" t="n"/>
       <c r="L39" s="1" t="n"/>
-      <c r="M39" s="1" t="n"/>
+      <c r="M39" s="1" t="n">
+        <v/>
+      </c>
       <c r="N39" s="1" t="n"/>
     </row>
     <row r="40">
@@ -1742,11 +2222,15 @@
           <t>7</t>
         </is>
       </c>
-      <c r="B40" s="1" t="n">
-        <v>113.87</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>11</v>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>113.87</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D40" s="1" t="inlineStr">
         <is>
@@ -1763,22 +2247,42 @@
           <t>thru</t>
         </is>
       </c>
-      <c r="G40" s="1" t="n"/>
-      <c r="H40" s="1" t="n"/>
-      <c r="I40" s="1" t="n"/>
-      <c r="J40" s="1" t="n"/>
+      <c r="G40" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H40" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J40" s="1" t="n">
+        <v/>
+      </c>
       <c r="K40" s="1" t="n"/>
-      <c r="L40" s="1" t="n"/>
-      <c r="M40" s="1" t="n"/>
-      <c r="N40" s="1" t="n"/>
+      <c r="L40" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N40" s="1" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n"/>
-      <c r="B41" s="1" t="n">
-        <v>113.87</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>11</v>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>113.87</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
@@ -1798,19 +2302,27 @@
       <c r="G41" s="1" t="n"/>
       <c r="H41" s="1" t="n"/>
       <c r="I41" s="1" t="n"/>
-      <c r="J41" s="1" t="n"/>
+      <c r="J41" s="1" t="n">
+        <v/>
+      </c>
       <c r="K41" s="1" t="n"/>
       <c r="L41" s="1" t="n"/>
-      <c r="M41" s="1" t="n"/>
+      <c r="M41" s="1" t="n">
+        <v/>
+      </c>
       <c r="N41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n"/>
-      <c r="B42" s="1" t="n">
-        <v>113.87</v>
-      </c>
-      <c r="C42" s="1" t="n">
-        <v>11</v>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>113.87</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D42" s="1" t="inlineStr">
         <is>
@@ -1830,19 +2342,27 @@
       <c r="G42" s="1" t="n"/>
       <c r="H42" s="1" t="n"/>
       <c r="I42" s="1" t="n"/>
-      <c r="J42" s="1" t="n"/>
+      <c r="J42" s="1" t="n">
+        <v/>
+      </c>
       <c r="K42" s="1" t="n"/>
       <c r="L42" s="1" t="n"/>
-      <c r="M42" s="1" t="n"/>
+      <c r="M42" s="1" t="n">
+        <v/>
+      </c>
       <c r="N42" s="1" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
-      <c r="B43" s="1" t="n">
-        <v>193.7</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>19</v>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>193.7</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="D43" s="1" t="inlineStr">
         <is>
@@ -1862,19 +2382,27 @@
       <c r="G43" s="1" t="n"/>
       <c r="H43" s="1" t="n"/>
       <c r="I43" s="1" t="n"/>
-      <c r="J43" s="1" t="n"/>
+      <c r="J43" s="1" t="n">
+        <v/>
+      </c>
       <c r="K43" s="1" t="n"/>
       <c r="L43" s="1" t="n"/>
-      <c r="M43" s="1" t="n"/>
+      <c r="M43" s="1" t="n">
+        <v/>
+      </c>
       <c r="N43" s="1" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n"/>
-      <c r="B44" s="1" t="n">
-        <v>193.7</v>
-      </c>
-      <c r="C44" s="1" t="n">
-        <v>19</v>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>193.7</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="D44" s="1" t="inlineStr">
         <is>
@@ -1894,19 +2422,27 @@
       <c r="G44" s="1" t="n"/>
       <c r="H44" s="1" t="n"/>
       <c r="I44" s="1" t="n"/>
-      <c r="J44" s="1" t="n"/>
+      <c r="J44" s="1" t="n">
+        <v/>
+      </c>
       <c r="K44" s="1" t="n"/>
       <c r="L44" s="1" t="n"/>
-      <c r="M44" s="1" t="n"/>
+      <c r="M44" s="1" t="n">
+        <v/>
+      </c>
       <c r="N44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
-      <c r="B45" s="1" t="n">
-        <v>193.7</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>19</v>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>193.7</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
       <c r="D45" s="1" t="inlineStr">
         <is>
@@ -1926,19 +2462,27 @@
       <c r="G45" s="1" t="n"/>
       <c r="H45" s="1" t="n"/>
       <c r="I45" s="1" t="n"/>
-      <c r="J45" s="1" t="n"/>
+      <c r="J45" s="1" t="n">
+        <v/>
+      </c>
       <c r="K45" s="1" t="n"/>
       <c r="L45" s="1" t="n"/>
-      <c r="M45" s="1" t="n"/>
+      <c r="M45" s="1" t="n">
+        <v/>
+      </c>
       <c r="N45" s="1" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
-      <c r="B46" s="1" t="n">
-        <v>294.04</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>29</v>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>294.04</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D46" s="1" t="inlineStr">
         <is>
@@ -1958,19 +2502,27 @@
       <c r="G46" s="1" t="n"/>
       <c r="H46" s="1" t="n"/>
       <c r="I46" s="1" t="n"/>
-      <c r="J46" s="1" t="n"/>
+      <c r="J46" s="1" t="n">
+        <v/>
+      </c>
       <c r="K46" s="1" t="n"/>
       <c r="L46" s="1" t="n"/>
-      <c r="M46" s="1" t="n"/>
+      <c r="M46" s="1" t="n">
+        <v/>
+      </c>
       <c r="N46" s="1" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n"/>
-      <c r="B47" s="1" t="n">
-        <v>294.04</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>29</v>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>294.04</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
@@ -1990,10 +2542,14 @@
       <c r="G47" s="1" t="n"/>
       <c r="H47" s="1" t="n"/>
       <c r="I47" s="1" t="n"/>
-      <c r="J47" s="1" t="n"/>
+      <c r="J47" s="1" t="n">
+        <v/>
+      </c>
       <c r="K47" s="1" t="n"/>
       <c r="L47" s="1" t="n"/>
-      <c r="M47" s="1" t="n"/>
+      <c r="M47" s="1" t="n">
+        <v/>
+      </c>
       <c r="N47" s="1" t="n"/>
     </row>
     <row r="48">
@@ -2002,11 +2558,15 @@
           <t>8</t>
         </is>
       </c>
-      <c r="B48" s="1" t="n">
-        <v>50.76</v>
-      </c>
-      <c r="C48" s="1" t="n">
-        <v>5</v>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>50.76</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="D48" s="1" t="inlineStr">
         <is>
@@ -2023,22 +2583,54 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G48" s="1" t="n"/>
-      <c r="H48" s="1" t="n"/>
-      <c r="I48" s="1" t="n"/>
-      <c r="J48" s="1" t="n"/>
+      <c r="G48" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+I75N_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H48" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I48" s="1" t="inlineStr">
+        <is>
+          <t>0414) Shallowford Rd &amp; I-75 NB</t>
+        </is>
+      </c>
+      <c r="J48" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
       <c r="K48" s="1" t="n"/>
-      <c r="L48" s="1" t="n"/>
-      <c r="M48" s="1" t="n"/>
-      <c r="N48" s="1" t="n"/>
+      <c r="L48" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="M48" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="N48" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
-      <c r="B49" s="1" t="n">
-        <v>50.76</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>5</v>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>50.76</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="D49" s="1" t="inlineStr">
         <is>
@@ -2058,19 +2650,31 @@
       <c r="G49" s="1" t="n"/>
       <c r="H49" s="1" t="n"/>
       <c r="I49" s="1" t="n"/>
-      <c r="J49" s="1" t="n"/>
+      <c r="J49" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="K49" s="1" t="n"/>
       <c r="L49" s="1" t="n"/>
-      <c r="M49" s="1" t="n"/>
+      <c r="M49" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="N49" s="1" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
-      <c r="B50" s="1" t="n">
-        <v>50.76</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>5</v>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>50.76</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="D50" s="1" t="inlineStr">
         <is>
@@ -2090,19 +2694,31 @@
       <c r="G50" s="1" t="n"/>
       <c r="H50" s="1" t="n"/>
       <c r="I50" s="1" t="n"/>
-      <c r="J50" s="1" t="n"/>
+      <c r="J50" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="K50" s="1" t="n"/>
       <c r="L50" s="1" t="n"/>
-      <c r="M50" s="1" t="n"/>
+      <c r="M50" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="N50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="n">
-        <v>114.36</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <v>11</v>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>114.36</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D51" s="1" t="inlineStr">
         <is>
@@ -2122,19 +2738,31 @@
       <c r="G51" s="1" t="n"/>
       <c r="H51" s="1" t="n"/>
       <c r="I51" s="1" t="n"/>
-      <c r="J51" s="1" t="n"/>
+      <c r="J51" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="K51" s="1" t="n"/>
       <c r="L51" s="1" t="n"/>
-      <c r="M51" s="1" t="n"/>
+      <c r="M51" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="N51" s="1" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n"/>
-      <c r="B52" s="1" t="n">
-        <v>114.36</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>11</v>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>114.36</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D52" s="1" t="inlineStr">
         <is>
@@ -2154,19 +2782,31 @@
       <c r="G52" s="1" t="n"/>
       <c r="H52" s="1" t="n"/>
       <c r="I52" s="1" t="n"/>
-      <c r="J52" s="1" t="n"/>
+      <c r="J52" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K52" s="1" t="n"/>
       <c r="L52" s="1" t="n"/>
-      <c r="M52" s="1" t="n"/>
+      <c r="M52" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N52" s="1" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n"/>
-      <c r="B53" s="1" t="n">
-        <v>114.36</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>11</v>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>114.36</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D53" s="1" t="inlineStr">
         <is>
@@ -2186,19 +2826,31 @@
       <c r="G53" s="1" t="n"/>
       <c r="H53" s="1" t="n"/>
       <c r="I53" s="1" t="n"/>
-      <c r="J53" s="1" t="n"/>
+      <c r="J53" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K53" s="1" t="n"/>
       <c r="L53" s="1" t="n"/>
-      <c r="M53" s="1" t="n"/>
+      <c r="M53" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="N53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n"/>
-      <c r="B54" s="1" t="n">
-        <v>296.65</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>30</v>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>296.65</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="D54" s="1" t="inlineStr">
         <is>
@@ -2218,19 +2870,31 @@
       <c r="G54" s="1" t="n"/>
       <c r="H54" s="1" t="n"/>
       <c r="I54" s="1" t="n"/>
-      <c r="J54" s="1" t="n"/>
+      <c r="J54" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K54" s="1" t="n"/>
       <c r="L54" s="1" t="n"/>
-      <c r="M54" s="1" t="n"/>
+      <c r="M54" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="N54" s="1" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n"/>
-      <c r="B55" s="1" t="n">
-        <v>296.65</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>30</v>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>296.65</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="D55" s="1" t="inlineStr">
         <is>
@@ -2250,10 +2914,18 @@
       <c r="G55" s="1" t="n"/>
       <c r="H55" s="1" t="n"/>
       <c r="I55" s="1" t="n"/>
-      <c r="J55" s="1" t="n"/>
+      <c r="J55" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="K55" s="1" t="n"/>
       <c r="L55" s="1" t="n"/>
-      <c r="M55" s="1" t="n"/>
+      <c r="M55" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="N55" s="1" t="n"/>
     </row>
     <row r="56">
@@ -2262,11 +2934,15 @@
           <t>9</t>
         </is>
       </c>
-      <c r="B56" s="1" t="n">
-        <v>111.5</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>11</v>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>111.5</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D56" s="1" t="inlineStr">
         <is>
@@ -2283,22 +2959,54 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G56" s="1" t="n"/>
-      <c r="H56" s="1" t="n"/>
-      <c r="I56" s="1" t="n"/>
-      <c r="J56" s="1" t="n"/>
+      <c r="G56" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+I75S_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H56" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I56" s="1" t="inlineStr">
+        <is>
+          <t>0413) Shallowford Rd &amp; I-75 SB</t>
+        </is>
+      </c>
+      <c r="J56" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="K56" s="1" t="n"/>
-      <c r="L56" s="1" t="n"/>
-      <c r="M56" s="1" t="n"/>
-      <c r="N56" s="1" t="n"/>
+      <c r="L56" s="1" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M56" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
+      <c r="N56" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n"/>
-      <c r="B57" s="1" t="n">
-        <v>111.5</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>11</v>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>111.5</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D57" s="1" t="inlineStr">
         <is>
@@ -2318,19 +3026,31 @@
       <c r="G57" s="1" t="n"/>
       <c r="H57" s="1" t="n"/>
       <c r="I57" s="1" t="n"/>
-      <c r="J57" s="1" t="n"/>
+      <c r="J57" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K57" s="1" t="n"/>
       <c r="L57" s="1" t="n"/>
-      <c r="M57" s="1" t="n"/>
+      <c r="M57" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N57" s="1" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n"/>
-      <c r="B58" s="1" t="n">
-        <v>235.09</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>24</v>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>235.09</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="D58" s="1" t="inlineStr">
         <is>
@@ -2350,19 +3070,31 @@
       <c r="G58" s="1" t="n"/>
       <c r="H58" s="1" t="n"/>
       <c r="I58" s="1" t="n"/>
-      <c r="J58" s="1" t="n"/>
+      <c r="J58" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K58" s="1" t="n"/>
       <c r="L58" s="1" t="n"/>
-      <c r="M58" s="1" t="n"/>
+      <c r="M58" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="N58" s="1" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n"/>
-      <c r="B59" s="1" t="n">
-        <v>235.09</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>24</v>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>235.09</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="D59" s="1" t="inlineStr">
         <is>
@@ -2382,19 +3114,31 @@
       <c r="G59" s="1" t="n"/>
       <c r="H59" s="1" t="n"/>
       <c r="I59" s="1" t="n"/>
-      <c r="J59" s="1" t="n"/>
+      <c r="J59" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K59" s="1" t="n"/>
       <c r="L59" s="1" t="n"/>
-      <c r="M59" s="1" t="n"/>
+      <c r="M59" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="N59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n"/>
-      <c r="B60" s="1" t="n">
-        <v>235.09</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>24</v>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>235.09</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="D60" s="1" t="inlineStr">
         <is>
@@ -2414,19 +3158,31 @@
       <c r="G60" s="1" t="n"/>
       <c r="H60" s="1" t="n"/>
       <c r="I60" s="1" t="n"/>
-      <c r="J60" s="1" t="n"/>
+      <c r="J60" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="K60" s="1" t="n"/>
       <c r="L60" s="1" t="n"/>
-      <c r="M60" s="1" t="n"/>
+      <c r="M60" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="N60" s="1" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n"/>
-      <c r="B61" s="1" t="n">
-        <v>291.99</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>29</v>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>291.99</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D61" s="1" t="inlineStr">
         <is>
@@ -2446,19 +3202,31 @@
       <c r="G61" s="1" t="n"/>
       <c r="H61" s="1" t="n"/>
       <c r="I61" s="1" t="n"/>
-      <c r="J61" s="1" t="n"/>
+      <c r="J61" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="K61" s="1" t="n"/>
       <c r="L61" s="1" t="n"/>
-      <c r="M61" s="1" t="n"/>
+      <c r="M61" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="N61" s="1" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n"/>
-      <c r="B62" s="1" t="n">
-        <v>291.99</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>29</v>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>291.99</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D62" s="1" t="inlineStr">
         <is>
@@ -2478,19 +3246,31 @@
       <c r="G62" s="1" t="n"/>
       <c r="H62" s="1" t="n"/>
       <c r="I62" s="1" t="n"/>
-      <c r="J62" s="1" t="n"/>
+      <c r="J62" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="K62" s="1" t="n"/>
       <c r="L62" s="1" t="n"/>
-      <c r="M62" s="1" t="n"/>
+      <c r="M62" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="N62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n"/>
-      <c r="B63" s="1" t="n">
-        <v>291.99</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>29</v>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>291.99</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D63" s="1" t="inlineStr">
         <is>
@@ -2510,10 +3290,18 @@
       <c r="G63" s="1" t="n"/>
       <c r="H63" s="1" t="n"/>
       <c r="I63" s="1" t="n"/>
-      <c r="J63" s="1" t="n"/>
+      <c r="J63" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="K63" s="1" t="n"/>
       <c r="L63" s="1" t="n"/>
-      <c r="M63" s="1" t="n"/>
+      <c r="M63" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="N63" s="1" t="n"/>
     </row>
     <row r="64">
@@ -2522,11 +3310,15 @@
           <t>10</t>
         </is>
       </c>
-      <c r="B64" s="1" t="n">
-        <v>25.84</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>3</v>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>25.84</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="D64" s="1" t="inlineStr">
         <is>
@@ -2543,22 +3335,54 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G64" s="1" t="n"/>
-      <c r="H64" s="1" t="n"/>
-      <c r="I64" s="1" t="n"/>
-      <c r="J64" s="1" t="n"/>
+      <c r="G64" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+Napier_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H64" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I64" s="1" t="inlineStr">
+        <is>
+          <t>0415) Shallowford Rd &amp; Napier Rd / Hamilton Place Blvd</t>
+        </is>
+      </c>
+      <c r="J64" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
       <c r="K64" s="1" t="n"/>
-      <c r="L64" s="1" t="n"/>
-      <c r="M64" s="1" t="n"/>
-      <c r="N64" s="1" t="n"/>
+      <c r="L64" s="1" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="M64" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="N64" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n"/>
-      <c r="B65" s="1" t="n">
-        <v>25.84</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>3</v>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>25.84</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="D65" s="1" t="inlineStr">
         <is>
@@ -2578,19 +3402,31 @@
       <c r="G65" s="1" t="n"/>
       <c r="H65" s="1" t="n"/>
       <c r="I65" s="1" t="n"/>
-      <c r="J65" s="1" t="n"/>
+      <c r="J65" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="K65" s="1" t="n"/>
       <c r="L65" s="1" t="n"/>
-      <c r="M65" s="1" t="n"/>
+      <c r="M65" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="N65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n"/>
-      <c r="B66" s="1" t="n">
-        <v>25.84</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>3</v>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>25.84</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="D66" s="1" t="inlineStr">
         <is>
@@ -2610,19 +3446,31 @@
       <c r="G66" s="1" t="n"/>
       <c r="H66" s="1" t="n"/>
       <c r="I66" s="1" t="n"/>
-      <c r="J66" s="1" t="n"/>
+      <c r="J66" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="K66" s="1" t="n"/>
       <c r="L66" s="1" t="n"/>
-      <c r="M66" s="1" t="n"/>
+      <c r="M66" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="N66" s="1" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n"/>
-      <c r="B67" s="1" t="n">
-        <v>25.84</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>3</v>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>25.84</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
       <c r="D67" s="1" t="inlineStr">
         <is>
@@ -2642,19 +3490,31 @@
       <c r="G67" s="1" t="n"/>
       <c r="H67" s="1" t="n"/>
       <c r="I67" s="1" t="n"/>
-      <c r="J67" s="1" t="n"/>
+      <c r="J67" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="K67" s="1" t="n"/>
       <c r="L67" s="1" t="n"/>
-      <c r="M67" s="1" t="n"/>
+      <c r="M67" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="N67" s="1" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n"/>
-      <c r="B68" s="1" t="n">
-        <v>116.65</v>
-      </c>
-      <c r="C68" s="1" t="n">
-        <v>12</v>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>116.65</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="D68" s="1" t="inlineStr">
         <is>
@@ -2674,19 +3534,31 @@
       <c r="G68" s="1" t="n"/>
       <c r="H68" s="1" t="n"/>
       <c r="I68" s="1" t="n"/>
-      <c r="J68" s="1" t="n"/>
+      <c r="J68" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="K68" s="1" t="n"/>
       <c r="L68" s="1" t="n"/>
-      <c r="M68" s="1" t="n"/>
+      <c r="M68" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="N68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n"/>
-      <c r="B69" s="1" t="n">
-        <v>116.65</v>
-      </c>
-      <c r="C69" s="1" t="n">
-        <v>12</v>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>116.65</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="D69" s="1" t="inlineStr">
         <is>
@@ -2706,19 +3578,31 @@
       <c r="G69" s="1" t="n"/>
       <c r="H69" s="1" t="n"/>
       <c r="I69" s="1" t="n"/>
-      <c r="J69" s="1" t="n"/>
+      <c r="J69" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K69" s="1" t="n"/>
       <c r="L69" s="1" t="n"/>
-      <c r="M69" s="1" t="n"/>
+      <c r="M69" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N69" s="1" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n"/>
-      <c r="B70" s="1" t="n">
-        <v>116.65</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>12</v>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>116.65</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="D70" s="1" t="inlineStr">
         <is>
@@ -2738,19 +3622,31 @@
       <c r="G70" s="1" t="n"/>
       <c r="H70" s="1" t="n"/>
       <c r="I70" s="1" t="n"/>
-      <c r="J70" s="1" t="n"/>
+      <c r="J70" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K70" s="1" t="n"/>
       <c r="L70" s="1" t="n"/>
-      <c r="M70" s="1" t="n"/>
+      <c r="M70" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="N70" s="1" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n"/>
-      <c r="B71" s="1" t="n">
-        <v>116.65</v>
-      </c>
-      <c r="C71" s="1" t="n">
-        <v>12</v>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>116.65</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="D71" s="1" t="inlineStr">
         <is>
@@ -2770,19 +3666,31 @@
       <c r="G71" s="1" t="n"/>
       <c r="H71" s="1" t="n"/>
       <c r="I71" s="1" t="n"/>
-      <c r="J71" s="1" t="n"/>
+      <c r="J71" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K71" s="1" t="n"/>
       <c r="L71" s="1" t="n"/>
-      <c r="M71" s="1" t="n"/>
+      <c r="M71" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="N71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n"/>
-      <c r="B72" s="1" t="n">
-        <v>202.48</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>20</v>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>202.48</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D72" s="1" t="inlineStr">
         <is>
@@ -2802,19 +3710,31 @@
       <c r="G72" s="1" t="n"/>
       <c r="H72" s="1" t="n"/>
       <c r="I72" s="1" t="n"/>
-      <c r="J72" s="1" t="n"/>
+      <c r="J72" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="K72" s="1" t="n"/>
       <c r="L72" s="1" t="n"/>
-      <c r="M72" s="1" t="n"/>
+      <c r="M72" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="N72" s="1" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n"/>
-      <c r="B73" s="1" t="n">
-        <v>202.48</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>20</v>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>202.48</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D73" s="1" t="inlineStr">
         <is>
@@ -2834,19 +3754,31 @@
       <c r="G73" s="1" t="n"/>
       <c r="H73" s="1" t="n"/>
       <c r="I73" s="1" t="n"/>
-      <c r="J73" s="1" t="n"/>
+      <c r="J73" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="K73" s="1" t="n"/>
       <c r="L73" s="1" t="n"/>
-      <c r="M73" s="1" t="n"/>
+      <c r="M73" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="N73" s="1" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n"/>
-      <c r="B74" s="1" t="n">
-        <v>202.48</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>20</v>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>202.48</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D74" s="1" t="inlineStr">
         <is>
@@ -2866,19 +3798,31 @@
       <c r="G74" s="1" t="n"/>
       <c r="H74" s="1" t="n"/>
       <c r="I74" s="1" t="n"/>
-      <c r="J74" s="1" t="n"/>
+      <c r="J74" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="K74" s="1" t="n"/>
       <c r="L74" s="1" t="n"/>
-      <c r="M74" s="1" t="n"/>
+      <c r="M74" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="N74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n"/>
-      <c r="B75" s="1" t="n">
-        <v>202.48</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>20</v>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>202.48</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D75" s="1" t="inlineStr">
         <is>
@@ -2898,19 +3842,31 @@
       <c r="G75" s="1" t="n"/>
       <c r="H75" s="1" t="n"/>
       <c r="I75" s="1" t="n"/>
-      <c r="J75" s="1" t="n"/>
+      <c r="J75" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="K75" s="1" t="n"/>
       <c r="L75" s="1" t="n"/>
-      <c r="M75" s="1" t="n"/>
+      <c r="M75" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="N75" s="1" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n"/>
-      <c r="B76" s="1" t="n">
-        <v>294.22</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>29</v>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>294.22</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D76" s="1" t="inlineStr">
         <is>
@@ -2930,19 +3886,31 @@
       <c r="G76" s="1" t="n"/>
       <c r="H76" s="1" t="n"/>
       <c r="I76" s="1" t="n"/>
-      <c r="J76" s="1" t="n"/>
+      <c r="J76" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="K76" s="1" t="n"/>
       <c r="L76" s="1" t="n"/>
-      <c r="M76" s="1" t="n"/>
+      <c r="M76" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="N76" s="1" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n"/>
-      <c r="B77" s="1" t="n">
-        <v>294.22</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>29</v>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t>294.22</t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D77" s="1" t="inlineStr">
         <is>
@@ -2962,19 +3930,31 @@
       <c r="G77" s="1" t="n"/>
       <c r="H77" s="1" t="n"/>
       <c r="I77" s="1" t="n"/>
-      <c r="J77" s="1" t="n"/>
+      <c r="J77" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="K77" s="1" t="n"/>
       <c r="L77" s="1" t="n"/>
-      <c r="M77" s="1" t="n"/>
+      <c r="M77" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="N77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n"/>
-      <c r="B78" s="1" t="n">
-        <v>294.22</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>29</v>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t>294.22</t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D78" s="1" t="inlineStr">
         <is>
@@ -2994,19 +3974,31 @@
       <c r="G78" s="1" t="n"/>
       <c r="H78" s="1" t="n"/>
       <c r="I78" s="1" t="n"/>
-      <c r="J78" s="1" t="n"/>
+      <c r="J78" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="K78" s="1" t="n"/>
       <c r="L78" s="1" t="n"/>
-      <c r="M78" s="1" t="n"/>
+      <c r="M78" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="N78" s="1" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n"/>
-      <c r="B79" s="1" t="n">
-        <v>294.22</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>29</v>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>294.22</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D79" s="1" t="inlineStr">
         <is>
@@ -3026,10 +4018,18 @@
       <c r="G79" s="1" t="n"/>
       <c r="H79" s="1" t="n"/>
       <c r="I79" s="1" t="n"/>
-      <c r="J79" s="1" t="n"/>
+      <c r="J79" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="K79" s="1" t="n"/>
       <c r="L79" s="1" t="n"/>
-      <c r="M79" s="1" t="n"/>
+      <c r="M79" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="N79" s="1" t="n"/>
     </row>
     <row r="80">
@@ -3038,11 +4038,15 @@
           <t>11</t>
         </is>
       </c>
-      <c r="B80" s="1" t="n">
-        <v>22.95</v>
-      </c>
-      <c r="C80" s="1" t="n">
-        <v>2</v>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>22.95</t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D80" s="1" t="inlineStr">
         <is>
@@ -3059,22 +4063,42 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G80" s="1" t="n"/>
-      <c r="H80" s="1" t="n"/>
-      <c r="I80" s="1" t="n"/>
-      <c r="J80" s="1" t="n"/>
+      <c r="G80" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H80" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J80" s="1" t="n">
+        <v/>
+      </c>
       <c r="K80" s="1" t="n"/>
-      <c r="L80" s="1" t="n"/>
-      <c r="M80" s="1" t="n"/>
-      <c r="N80" s="1" t="n"/>
+      <c r="L80" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M80" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N80" s="1" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n"/>
-      <c r="B81" s="1" t="n">
-        <v>113.22</v>
-      </c>
-      <c r="C81" s="1" t="n">
-        <v>11</v>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t>113.22</t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D81" s="1" t="inlineStr">
         <is>
@@ -3094,19 +4118,27 @@
       <c r="G81" s="1" t="n"/>
       <c r="H81" s="1" t="n"/>
       <c r="I81" s="1" t="n"/>
-      <c r="J81" s="1" t="n"/>
+      <c r="J81" s="1" t="n">
+        <v/>
+      </c>
       <c r="K81" s="1" t="n"/>
       <c r="L81" s="1" t="n"/>
-      <c r="M81" s="1" t="n"/>
+      <c r="M81" s="1" t="n">
+        <v/>
+      </c>
       <c r="N81" s="1" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n"/>
-      <c r="B82" s="1" t="n">
-        <v>113.22</v>
-      </c>
-      <c r="C82" s="1" t="n">
-        <v>11</v>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t>113.22</t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D82" s="1" t="inlineStr">
         <is>
@@ -3126,19 +4158,27 @@
       <c r="G82" s="1" t="n"/>
       <c r="H82" s="1" t="n"/>
       <c r="I82" s="1" t="n"/>
-      <c r="J82" s="1" t="n"/>
+      <c r="J82" s="1" t="n">
+        <v/>
+      </c>
       <c r="K82" s="1" t="n"/>
       <c r="L82" s="1" t="n"/>
-      <c r="M82" s="1" t="n"/>
+      <c r="M82" s="1" t="n">
+        <v/>
+      </c>
       <c r="N82" s="1" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n"/>
-      <c r="B83" s="1" t="n">
-        <v>113.22</v>
-      </c>
-      <c r="C83" s="1" t="n">
-        <v>11</v>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>113.22</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D83" s="1" t="inlineStr">
         <is>
@@ -3158,19 +4198,27 @@
       <c r="G83" s="1" t="n"/>
       <c r="H83" s="1" t="n"/>
       <c r="I83" s="1" t="n"/>
-      <c r="J83" s="1" t="n"/>
+      <c r="J83" s="1" t="n">
+        <v/>
+      </c>
       <c r="K83" s="1" t="n"/>
       <c r="L83" s="1" t="n"/>
-      <c r="M83" s="1" t="n"/>
+      <c r="M83" s="1" t="n">
+        <v/>
+      </c>
       <c r="N83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n"/>
-      <c r="B84" s="1" t="n">
-        <v>291.47</v>
-      </c>
-      <c r="C84" s="1" t="n">
-        <v>29</v>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t>291.47</t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D84" s="1" t="inlineStr">
         <is>
@@ -3190,19 +4238,27 @@
       <c r="G84" s="1" t="n"/>
       <c r="H84" s="1" t="n"/>
       <c r="I84" s="1" t="n"/>
-      <c r="J84" s="1" t="n"/>
+      <c r="J84" s="1" t="n">
+        <v/>
+      </c>
       <c r="K84" s="1" t="n"/>
       <c r="L84" s="1" t="n"/>
-      <c r="M84" s="1" t="n"/>
+      <c r="M84" s="1" t="n">
+        <v/>
+      </c>
       <c r="N84" s="1" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n"/>
-      <c r="B85" s="1" t="n">
-        <v>291.47</v>
-      </c>
-      <c r="C85" s="1" t="n">
-        <v>29</v>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>291.47</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D85" s="1" t="inlineStr">
         <is>
@@ -3222,19 +4278,27 @@
       <c r="G85" s="1" t="n"/>
       <c r="H85" s="1" t="n"/>
       <c r="I85" s="1" t="n"/>
-      <c r="J85" s="1" t="n"/>
+      <c r="J85" s="1" t="n">
+        <v/>
+      </c>
       <c r="K85" s="1" t="n"/>
       <c r="L85" s="1" t="n"/>
-      <c r="M85" s="1" t="n"/>
+      <c r="M85" s="1" t="n">
+        <v/>
+      </c>
       <c r="N85" s="1" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n"/>
-      <c r="B86" s="1" t="n">
-        <v>291.47</v>
-      </c>
-      <c r="C86" s="1" t="n">
-        <v>29</v>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>291.47</t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D86" s="1" t="inlineStr">
         <is>
@@ -3254,10 +4318,14 @@
       <c r="G86" s="1" t="n"/>
       <c r="H86" s="1" t="n"/>
       <c r="I86" s="1" t="n"/>
-      <c r="J86" s="1" t="n"/>
+      <c r="J86" s="1" t="n">
+        <v/>
+      </c>
       <c r="K86" s="1" t="n"/>
       <c r="L86" s="1" t="n"/>
-      <c r="M86" s="1" t="n"/>
+      <c r="M86" s="1" t="n">
+        <v/>
+      </c>
       <c r="N86" s="1" t="n"/>
     </row>
     <row r="87">
@@ -3266,11 +4334,15 @@
           <t>12</t>
         </is>
       </c>
-      <c r="B87" s="1" t="n">
-        <v>23.34</v>
-      </c>
-      <c r="C87" s="1" t="n">
-        <v>2</v>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>23.34</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D87" s="1" t="inlineStr">
         <is>
@@ -3287,22 +4359,54 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G87" s="1" t="n"/>
-      <c r="H87" s="1" t="n"/>
-      <c r="I87" s="1" t="n"/>
-      <c r="J87" s="1" t="n"/>
+      <c r="G87" s="1" t="inlineStr">
+        <is>
+          <t>Shallowford+Amin_07112023.xls</t>
+        </is>
+      </c>
+      <c r="H87" s="1" t="inlineStr">
+        <is>
+          <t>7/11/2023</t>
+        </is>
+      </c>
+      <c r="I87" s="1" t="inlineStr">
+        <is>
+          <t>0412) Shallowford Rd &amp; Shallowford Village Dr / Amin Dr</t>
+        </is>
+      </c>
+      <c r="J87" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
       <c r="K87" s="1" t="n"/>
-      <c r="L87" s="1" t="n"/>
-      <c r="M87" s="1" t="n"/>
-      <c r="N87" s="1" t="n"/>
+      <c r="L87" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="M87" s="1" t="inlineStr">
+        <is>
+          <t>NBR</t>
+        </is>
+      </c>
+      <c r="N87" s="1" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n"/>
-      <c r="B88" s="1" t="n">
-        <v>23.34</v>
-      </c>
-      <c r="C88" s="1" t="n">
-        <v>2</v>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>23.34</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D88" s="1" t="inlineStr">
         <is>
@@ -3322,19 +4426,31 @@
       <c r="G88" s="1" t="n"/>
       <c r="H88" s="1" t="n"/>
       <c r="I88" s="1" t="n"/>
-      <c r="J88" s="1" t="n"/>
+      <c r="J88" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="K88" s="1" t="n"/>
       <c r="L88" s="1" t="n"/>
-      <c r="M88" s="1" t="n"/>
+      <c r="M88" s="1" t="inlineStr">
+        <is>
+          <t>NBT</t>
+        </is>
+      </c>
       <c r="N88" s="1" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n"/>
-      <c r="B89" s="1" t="n">
-        <v>23.34</v>
-      </c>
-      <c r="C89" s="1" t="n">
-        <v>2</v>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>23.34</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D89" s="1" t="inlineStr">
         <is>
@@ -3354,19 +4470,31 @@
       <c r="G89" s="1" t="n"/>
       <c r="H89" s="1" t="n"/>
       <c r="I89" s="1" t="n"/>
-      <c r="J89" s="1" t="n"/>
+      <c r="J89" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="K89" s="1" t="n"/>
       <c r="L89" s="1" t="n"/>
-      <c r="M89" s="1" t="n"/>
+      <c r="M89" s="1" t="inlineStr">
+        <is>
+          <t>NBL</t>
+        </is>
+      </c>
       <c r="N89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n"/>
-      <c r="B90" s="1" t="n">
-        <v>23.34</v>
-      </c>
-      <c r="C90" s="1" t="n">
-        <v>2</v>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>23.34</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D90" s="1" t="inlineStr">
         <is>
@@ -3386,19 +4514,31 @@
       <c r="G90" s="1" t="n"/>
       <c r="H90" s="1" t="n"/>
       <c r="I90" s="1" t="n"/>
-      <c r="J90" s="1" t="n"/>
+      <c r="J90" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="K90" s="1" t="n"/>
       <c r="L90" s="1" t="n"/>
-      <c r="M90" s="1" t="n"/>
+      <c r="M90" s="1" t="inlineStr">
+        <is>
+          <t>NBU</t>
+        </is>
+      </c>
       <c r="N90" s="1" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n"/>
-      <c r="B91" s="1" t="n">
-        <v>114.28</v>
-      </c>
-      <c r="C91" s="1" t="n">
-        <v>11</v>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>114.28</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D91" s="1" t="inlineStr">
         <is>
@@ -3418,19 +4558,31 @@
       <c r="G91" s="1" t="n"/>
       <c r="H91" s="1" t="n"/>
       <c r="I91" s="1" t="n"/>
-      <c r="J91" s="1" t="n"/>
+      <c r="J91" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="K91" s="1" t="n"/>
       <c r="L91" s="1" t="n"/>
-      <c r="M91" s="1" t="n"/>
+      <c r="M91" s="1" t="inlineStr">
+        <is>
+          <t>EBR</t>
+        </is>
+      </c>
       <c r="N91" s="1" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n"/>
-      <c r="B92" s="1" t="n">
-        <v>114.28</v>
-      </c>
-      <c r="C92" s="1" t="n">
-        <v>11</v>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t>114.28</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D92" s="1" t="inlineStr">
         <is>
@@ -3450,19 +4602,31 @@
       <c r="G92" s="1" t="n"/>
       <c r="H92" s="1" t="n"/>
       <c r="I92" s="1" t="n"/>
-      <c r="J92" s="1" t="n"/>
+      <c r="J92" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="K92" s="1" t="n"/>
       <c r="L92" s="1" t="n"/>
-      <c r="M92" s="1" t="n"/>
+      <c r="M92" s="1" t="inlineStr">
+        <is>
+          <t>EBT</t>
+        </is>
+      </c>
       <c r="N92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n"/>
-      <c r="B93" s="1" t="n">
-        <v>114.28</v>
-      </c>
-      <c r="C93" s="1" t="n">
-        <v>11</v>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>114.28</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D93" s="1" t="inlineStr">
         <is>
@@ -3482,19 +4646,31 @@
       <c r="G93" s="1" t="n"/>
       <c r="H93" s="1" t="n"/>
       <c r="I93" s="1" t="n"/>
-      <c r="J93" s="1" t="n"/>
+      <c r="J93" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="K93" s="1" t="n"/>
       <c r="L93" s="1" t="n"/>
-      <c r="M93" s="1" t="n"/>
+      <c r="M93" s="1" t="inlineStr">
+        <is>
+          <t>EBL</t>
+        </is>
+      </c>
       <c r="N93" s="1" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n"/>
-      <c r="B94" s="1" t="n">
-        <v>114.28</v>
-      </c>
-      <c r="C94" s="1" t="n">
-        <v>11</v>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>114.28</t>
+        </is>
+      </c>
+      <c r="C94" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D94" s="1" t="inlineStr">
         <is>
@@ -3514,19 +4690,31 @@
       <c r="G94" s="1" t="n"/>
       <c r="H94" s="1" t="n"/>
       <c r="I94" s="1" t="n"/>
-      <c r="J94" s="1" t="n"/>
+      <c r="J94" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="K94" s="1" t="n"/>
       <c r="L94" s="1" t="n"/>
-      <c r="M94" s="1" t="n"/>
+      <c r="M94" s="1" t="inlineStr">
+        <is>
+          <t>EBU</t>
+        </is>
+      </c>
       <c r="N94" s="1" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n"/>
-      <c r="B95" s="1" t="n">
-        <v>201.4</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>20</v>
+      <c r="B95" s="1" t="inlineStr">
+        <is>
+          <t>201.4</t>
+        </is>
+      </c>
+      <c r="C95" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D95" s="1" t="inlineStr">
         <is>
@@ -3546,19 +4734,31 @@
       <c r="G95" s="1" t="n"/>
       <c r="H95" s="1" t="n"/>
       <c r="I95" s="1" t="n"/>
-      <c r="J95" s="1" t="n"/>
+      <c r="J95" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="K95" s="1" t="n"/>
       <c r="L95" s="1" t="n"/>
-      <c r="M95" s="1" t="n"/>
+      <c r="M95" s="1" t="inlineStr">
+        <is>
+          <t>SBR</t>
+        </is>
+      </c>
       <c r="N95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n"/>
-      <c r="B96" s="1" t="n">
-        <v>201.4</v>
-      </c>
-      <c r="C96" s="1" t="n">
-        <v>20</v>
+      <c r="B96" s="1" t="inlineStr">
+        <is>
+          <t>201.4</t>
+        </is>
+      </c>
+      <c r="C96" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D96" s="1" t="inlineStr">
         <is>
@@ -3578,19 +4778,31 @@
       <c r="G96" s="1" t="n"/>
       <c r="H96" s="1" t="n"/>
       <c r="I96" s="1" t="n"/>
-      <c r="J96" s="1" t="n"/>
+      <c r="J96" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="K96" s="1" t="n"/>
       <c r="L96" s="1" t="n"/>
-      <c r="M96" s="1" t="n"/>
+      <c r="M96" s="1" t="inlineStr">
+        <is>
+          <t>SBT</t>
+        </is>
+      </c>
       <c r="N96" s="1" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n"/>
-      <c r="B97" s="1" t="n">
-        <v>201.4</v>
-      </c>
-      <c r="C97" s="1" t="n">
-        <v>20</v>
+      <c r="B97" s="1" t="inlineStr">
+        <is>
+          <t>201.4</t>
+        </is>
+      </c>
+      <c r="C97" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D97" s="1" t="inlineStr">
         <is>
@@ -3610,19 +4822,31 @@
       <c r="G97" s="1" t="n"/>
       <c r="H97" s="1" t="n"/>
       <c r="I97" s="1" t="n"/>
-      <c r="J97" s="1" t="n"/>
+      <c r="J97" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="K97" s="1" t="n"/>
       <c r="L97" s="1" t="n"/>
-      <c r="M97" s="1" t="n"/>
+      <c r="M97" s="1" t="inlineStr">
+        <is>
+          <t>SBL</t>
+        </is>
+      </c>
       <c r="N97" s="1" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n"/>
-      <c r="B98" s="1" t="n">
-        <v>201.4</v>
-      </c>
-      <c r="C98" s="1" t="n">
-        <v>20</v>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t>201.4</t>
+        </is>
+      </c>
+      <c r="C98" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="D98" s="1" t="inlineStr">
         <is>
@@ -3642,19 +4866,31 @@
       <c r="G98" s="1" t="n"/>
       <c r="H98" s="1" t="n"/>
       <c r="I98" s="1" t="n"/>
-      <c r="J98" s="1" t="n"/>
+      <c r="J98" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="K98" s="1" t="n"/>
       <c r="L98" s="1" t="n"/>
-      <c r="M98" s="1" t="n"/>
+      <c r="M98" s="1" t="inlineStr">
+        <is>
+          <t>SBU</t>
+        </is>
+      </c>
       <c r="N98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n"/>
-      <c r="B99" s="1" t="n">
-        <v>293.24</v>
-      </c>
-      <c r="C99" s="1" t="n">
-        <v>29</v>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t>293.24</t>
+        </is>
+      </c>
+      <c r="C99" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D99" s="1" t="inlineStr">
         <is>
@@ -3674,19 +4910,31 @@
       <c r="G99" s="1" t="n"/>
       <c r="H99" s="1" t="n"/>
       <c r="I99" s="1" t="n"/>
-      <c r="J99" s="1" t="n"/>
+      <c r="J99" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="K99" s="1" t="n"/>
       <c r="L99" s="1" t="n"/>
-      <c r="M99" s="1" t="n"/>
+      <c r="M99" s="1" t="inlineStr">
+        <is>
+          <t>WBR</t>
+        </is>
+      </c>
       <c r="N99" s="1" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n"/>
-      <c r="B100" s="1" t="n">
-        <v>293.24</v>
-      </c>
-      <c r="C100" s="1" t="n">
-        <v>29</v>
+      <c r="B100" s="1" t="inlineStr">
+        <is>
+          <t>293.24</t>
+        </is>
+      </c>
+      <c r="C100" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D100" s="1" t="inlineStr">
         <is>
@@ -3706,19 +4954,31 @@
       <c r="G100" s="1" t="n"/>
       <c r="H100" s="1" t="n"/>
       <c r="I100" s="1" t="n"/>
-      <c r="J100" s="1" t="n"/>
+      <c r="J100" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="K100" s="1" t="n"/>
       <c r="L100" s="1" t="n"/>
-      <c r="M100" s="1" t="n"/>
+      <c r="M100" s="1" t="inlineStr">
+        <is>
+          <t>WBT</t>
+        </is>
+      </c>
       <c r="N100" s="1" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n"/>
-      <c r="B101" s="1" t="n">
-        <v>293.24</v>
-      </c>
-      <c r="C101" s="1" t="n">
-        <v>29</v>
+      <c r="B101" s="1" t="inlineStr">
+        <is>
+          <t>293.24</t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D101" s="1" t="inlineStr">
         <is>
@@ -3738,19 +4998,31 @@
       <c r="G101" s="1" t="n"/>
       <c r="H101" s="1" t="n"/>
       <c r="I101" s="1" t="n"/>
-      <c r="J101" s="1" t="n"/>
+      <c r="J101" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="K101" s="1" t="n"/>
       <c r="L101" s="1" t="n"/>
-      <c r="M101" s="1" t="n"/>
+      <c r="M101" s="1" t="inlineStr">
+        <is>
+          <t>WBL</t>
+        </is>
+      </c>
       <c r="N101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n"/>
-      <c r="B102" s="1" t="n">
-        <v>293.24</v>
-      </c>
-      <c r="C102" s="1" t="n">
-        <v>29</v>
+      <c r="B102" s="1" t="inlineStr">
+        <is>
+          <t>293.24</t>
+        </is>
+      </c>
+      <c r="C102" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D102" s="1" t="inlineStr">
         <is>
@@ -3770,10 +5042,18 @@
       <c r="G102" s="1" t="n"/>
       <c r="H102" s="1" t="n"/>
       <c r="I102" s="1" t="n"/>
-      <c r="J102" s="1" t="n"/>
+      <c r="J102" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="K102" s="1" t="n"/>
       <c r="L102" s="1" t="n"/>
-      <c r="M102" s="1" t="n"/>
+      <c r="M102" s="1" t="inlineStr">
+        <is>
+          <t>WBU</t>
+        </is>
+      </c>
       <c r="N102" s="1" t="n"/>
     </row>
     <row r="103">
@@ -3782,11 +5062,15 @@
           <t>18</t>
         </is>
       </c>
-      <c r="B103" s="1" t="n">
-        <v>24.02</v>
-      </c>
-      <c r="C103" s="1" t="n">
-        <v>2</v>
+      <c r="B103" s="1" t="inlineStr">
+        <is>
+          <t>24.02</t>
+        </is>
+      </c>
+      <c r="C103" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="D103" s="1" t="inlineStr">
         <is>
@@ -3803,22 +5087,42 @@
           <t>right</t>
         </is>
       </c>
-      <c r="G103" s="1" t="n"/>
-      <c r="H103" s="1" t="n"/>
-      <c r="I103" s="1" t="n"/>
-      <c r="J103" s="1" t="n"/>
+      <c r="G103" s="1" t="n">
+        <v/>
+      </c>
+      <c r="H103" s="1" t="n">
+        <v/>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v/>
+      </c>
+      <c r="J103" s="1" t="n">
+        <v/>
+      </c>
       <c r="K103" s="1" t="n"/>
-      <c r="L103" s="1" t="n"/>
-      <c r="M103" s="1" t="n"/>
-      <c r="N103" s="1" t="n"/>
+      <c r="L103" s="1" t="n">
+        <v/>
+      </c>
+      <c r="M103" s="1" t="n">
+        <v/>
+      </c>
+      <c r="N103" s="1" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n"/>
-      <c r="B104" s="1" t="n">
-        <v>114.26</v>
-      </c>
-      <c r="C104" s="1" t="n">
-        <v>11</v>
+      <c r="B104" s="1" t="inlineStr">
+        <is>
+          <t>114.26</t>
+        </is>
+      </c>
+      <c r="C104" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D104" s="1" t="inlineStr">
         <is>
@@ -3838,19 +5142,27 @@
       <c r="G104" s="1" t="n"/>
       <c r="H104" s="1" t="n"/>
       <c r="I104" s="1" t="n"/>
-      <c r="J104" s="1" t="n"/>
+      <c r="J104" s="1" t="n">
+        <v/>
+      </c>
       <c r="K104" s="1" t="n"/>
       <c r="L104" s="1" t="n"/>
-      <c r="M104" s="1" t="n"/>
+      <c r="M104" s="1" t="n">
+        <v/>
+      </c>
       <c r="N104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n"/>
-      <c r="B105" s="1" t="n">
-        <v>114.26</v>
-      </c>
-      <c r="C105" s="1" t="n">
-        <v>11</v>
+      <c r="B105" s="1" t="inlineStr">
+        <is>
+          <t>114.26</t>
+        </is>
+      </c>
+      <c r="C105" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
       <c r="D105" s="1" t="inlineStr">
         <is>
@@ -3870,19 +5182,27 @@
       <c r="G105" s="1" t="n"/>
       <c r="H105" s="1" t="n"/>
       <c r="I105" s="1" t="n"/>
-      <c r="J105" s="1" t="n"/>
+      <c r="J105" s="1" t="n">
+        <v/>
+      </c>
       <c r="K105" s="1" t="n"/>
       <c r="L105" s="1" t="n"/>
-      <c r="M105" s="1" t="n"/>
+      <c r="M105" s="1" t="n">
+        <v/>
+      </c>
       <c r="N105" s="1" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n"/>
-      <c r="B106" s="1" t="n">
-        <v>293.29</v>
-      </c>
-      <c r="C106" s="1" t="n">
-        <v>29</v>
+      <c r="B106" s="1" t="inlineStr">
+        <is>
+          <t>293.29</t>
+        </is>
+      </c>
+      <c r="C106" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
       <c r="D106" s="1" t="inlineStr">
         <is>
@@ -3902,10 +5222,14 @@
       <c r="G106" s="1" t="n"/>
       <c r="H106" s="1" t="n"/>
       <c r="I106" s="1" t="n"/>
-      <c r="J106" s="1" t="n"/>
+      <c r="J106" s="1" t="n">
+        <v/>
+      </c>
       <c r="K106" s="1" t="n"/>
       <c r="L106" s="1" t="n"/>
-      <c r="M106" s="1" t="n"/>
+      <c r="M106" s="1" t="n">
+        <v/>
+      </c>
       <c r="N106" s="1" t="n"/>
     </row>
   </sheetData>

</xml_diff>